<commit_message>
updated dataset with new data, changed figures and added analyses
</commit_message>
<xml_diff>
--- a/data/2021-11-17 _DetroitRiver_lab-analyses.xlsx
+++ b/data/2021-11-17 _DetroitRiver_lab-analyses.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sklem\Documents\Etudes\Trent\Xenopoulos lab\Projects\Lake Erie &amp; animal excretion\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://trentu-my.sharepoint.com/personal/sandraklemet_trentu_ca/Documents/Documents/Etudes/Trent/Xenopoulos lab/Projects/LakeErie_animal-excretion/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C8BF3FC-06BC-4E3E-A3F0-E9F8B77F733C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{7C8BF3FC-06BC-4E3E-A3F0-E9F8B77F733C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D9E71113-88D8-40CB-900B-19EDE952E276}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="490" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{C52185F6-50D3-4B58-B3B1-F9E06922E42E}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="3" xr2:uid="{C52185F6-50D3-4B58-B3B1-F9E06922E42E}"/>
   </bookViews>
   <sheets>
     <sheet name="SRP STD curve" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="NH4 STD curve" sheetId="2" r:id="rId3"/>
     <sheet name="NH4 samples" sheetId="3" r:id="rId4"/>
     <sheet name="TDP STD curve" sheetId="5" r:id="rId5"/>
+    <sheet name="TDP samples" sheetId="6" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'NH4 samples'!$A$1:$F$116</definedName>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="139">
   <si>
     <t>STDS</t>
   </si>
@@ -456,6 +457,9 @@
   </si>
   <si>
     <t>NH4 50% DILUTION (ug/L)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -11411,11 +11415,11 @@
         <v>3.3599999999999998E-2</v>
       </c>
       <c r="E2">
-        <f>AVERAGE(C2:D2)</f>
+        <f t="shared" ref="E2:E33" si="0">AVERAGE(C2:D2)</f>
         <v>3.3699999999999994E-2</v>
       </c>
       <c r="F2">
-        <f>980.61*E2+2.4087</f>
+        <f t="shared" ref="F2:F33" si="1">980.61*E2+2.4087</f>
         <v>35.455256999999996</v>
       </c>
     </row>
@@ -11433,11 +11437,11 @@
         <v>2.46E-2</v>
       </c>
       <c r="E3">
-        <f>AVERAGE(C3:D3)</f>
+        <f t="shared" si="0"/>
         <v>2.3449999999999999E-2</v>
       </c>
       <c r="F3">
-        <f>980.61*E3+2.4087</f>
+        <f t="shared" si="1"/>
         <v>25.404004499999999</v>
       </c>
     </row>
@@ -11455,11 +11459,11 @@
         <v>1.7500000000000002E-2</v>
       </c>
       <c r="E4">
-        <f>AVERAGE(C4:D4)</f>
+        <f t="shared" si="0"/>
         <v>1.6750000000000001E-2</v>
       </c>
       <c r="F4">
-        <f>980.61*E4+2.4087</f>
+        <f t="shared" si="1"/>
         <v>18.833917500000002</v>
       </c>
     </row>
@@ -11477,11 +11481,11 @@
         <v>1.77E-2</v>
       </c>
       <c r="E5">
-        <f>AVERAGE(C5:D5)</f>
+        <f t="shared" si="0"/>
         <v>1.4250000000000001E-2</v>
       </c>
       <c r="F5">
-        <f>980.61*E5+2.4087</f>
+        <f t="shared" si="1"/>
         <v>16.382392500000002</v>
       </c>
     </row>
@@ -11499,11 +11503,11 @@
         <v>1.2E-2</v>
       </c>
       <c r="E6">
-        <f>AVERAGE(C6:D6)</f>
+        <f t="shared" si="0"/>
         <v>1.115E-2</v>
       </c>
       <c r="F6">
-        <f>980.61*E6+2.4087</f>
+        <f t="shared" si="1"/>
         <v>13.342501499999999</v>
       </c>
     </row>
@@ -11521,11 +11525,11 @@
         <v>2.46E-2</v>
       </c>
       <c r="E7">
-        <f>AVERAGE(C7:D7)</f>
+        <f t="shared" si="0"/>
         <v>2.5649999999999999E-2</v>
       </c>
       <c r="F7">
-        <f>980.61*E7+2.4087</f>
+        <f t="shared" si="1"/>
         <v>27.561346499999999</v>
       </c>
     </row>
@@ -11543,11 +11547,11 @@
         <v>1.7100000000000001E-2</v>
       </c>
       <c r="E8">
-        <f>AVERAGE(C8:D8)</f>
+        <f t="shared" si="0"/>
         <v>1.78E-2</v>
       </c>
       <c r="F8">
-        <f>980.61*E8+2.4087</f>
+        <f t="shared" si="1"/>
         <v>19.863558000000001</v>
       </c>
     </row>
@@ -11565,11 +11569,11 @@
         <v>2.0899999999999998E-2</v>
       </c>
       <c r="E9">
-        <f>AVERAGE(C9:D9)</f>
+        <f t="shared" si="0"/>
         <v>2.3800000000000002E-2</v>
       </c>
       <c r="F9">
-        <f>980.61*E9+2.4087</f>
+        <f t="shared" si="1"/>
         <v>25.747218</v>
       </c>
     </row>
@@ -11587,11 +11591,11 @@
         <v>2.7799999999999998E-2</v>
       </c>
       <c r="E10">
-        <f>AVERAGE(C10:D10)</f>
+        <f t="shared" si="0"/>
         <v>2.9499999999999998E-2</v>
       </c>
       <c r="F10">
-        <f>980.61*E10+2.4087</f>
+        <f t="shared" si="1"/>
         <v>31.336694999999999</v>
       </c>
     </row>
@@ -11609,11 +11613,11 @@
         <v>3.5099999999999999E-2</v>
       </c>
       <c r="E11">
-        <f>AVERAGE(C11:D11)</f>
+        <f t="shared" si="0"/>
         <v>3.6749999999999998E-2</v>
       </c>
       <c r="F11">
-        <f>980.61*E11+2.4087</f>
+        <f t="shared" si="1"/>
         <v>38.4461175</v>
       </c>
     </row>
@@ -11631,11 +11635,11 @@
         <v>1.55E-2</v>
       </c>
       <c r="E12">
-        <f>AVERAGE(C12:D12)</f>
+        <f t="shared" si="0"/>
         <v>1.14E-2</v>
       </c>
       <c r="F12">
-        <f>980.61*E12+2.4087</f>
+        <f t="shared" si="1"/>
         <v>13.587654000000001</v>
       </c>
     </row>
@@ -11653,11 +11657,11 @@
         <v>4.5499999999999999E-2</v>
       </c>
       <c r="E13">
-        <f>AVERAGE(C13:D13)</f>
+        <f t="shared" si="0"/>
         <v>4.3450000000000003E-2</v>
       </c>
       <c r="F13">
-        <f>980.61*E13+2.4087</f>
+        <f t="shared" si="1"/>
         <v>45.016204500000008</v>
       </c>
     </row>
@@ -11675,11 +11679,11 @@
         <v>3.0099999999999998E-2</v>
       </c>
       <c r="E14">
-        <f>AVERAGE(C14:D14)</f>
+        <f t="shared" si="0"/>
         <v>2.7499999999999997E-2</v>
       </c>
       <c r="F14">
-        <f>980.61*E14+2.4087</f>
+        <f t="shared" si="1"/>
         <v>29.375474999999998</v>
       </c>
     </row>
@@ -11697,11 +11701,11 @@
         <v>2.87E-2</v>
       </c>
       <c r="E15">
-        <f>AVERAGE(C15:D15)</f>
+        <f t="shared" si="0"/>
         <v>2.9499999999999998E-2</v>
       </c>
       <c r="F15">
-        <f>980.61*E15+2.4087</f>
+        <f t="shared" si="1"/>
         <v>31.336694999999999</v>
       </c>
     </row>
@@ -11719,11 +11723,11 @@
         <v>1.8200000000000001E-2</v>
       </c>
       <c r="E16">
-        <f>AVERAGE(C16:D16)</f>
+        <f t="shared" si="0"/>
         <v>1.755E-2</v>
       </c>
       <c r="F16">
-        <f>980.61*E16+2.4087</f>
+        <f t="shared" si="1"/>
         <v>19.618405499999998</v>
       </c>
     </row>
@@ -11741,11 +11745,11 @@
         <v>1.2200000000000001E-2</v>
       </c>
       <c r="E17">
-        <f>AVERAGE(C17:D17)</f>
+        <f t="shared" si="0"/>
         <v>1.4600000000000002E-2</v>
       </c>
       <c r="F17">
-        <f>980.61*E17+2.4087</f>
+        <f t="shared" si="1"/>
         <v>16.725606000000003</v>
       </c>
     </row>
@@ -11763,11 +11767,11 @@
         <v>1.8499999999999999E-2</v>
       </c>
       <c r="E18">
-        <f>AVERAGE(C18:D18)</f>
+        <f t="shared" si="0"/>
         <v>1.5449999999999998E-2</v>
       </c>
       <c r="F18">
-        <f>980.61*E18+2.4087</f>
+        <f t="shared" si="1"/>
         <v>17.559124499999999</v>
       </c>
     </row>
@@ -11785,11 +11789,11 @@
         <v>2.2499999999999999E-2</v>
       </c>
       <c r="E19">
-        <f>AVERAGE(C19:D19)</f>
+        <f t="shared" si="0"/>
         <v>2.1600000000000001E-2</v>
       </c>
       <c r="F19">
-        <f>980.61*E19+2.4087</f>
+        <f t="shared" si="1"/>
         <v>23.589876</v>
       </c>
     </row>
@@ -11807,11 +11811,11 @@
         <v>1.3899999999999999E-2</v>
       </c>
       <c r="E20">
-        <f>AVERAGE(C20:D20)</f>
+        <f t="shared" si="0"/>
         <v>1.5099999999999999E-2</v>
       </c>
       <c r="F20">
-        <f>980.61*E20+2.4087</f>
+        <f t="shared" si="1"/>
         <v>17.215910999999998</v>
       </c>
     </row>
@@ -11829,11 +11833,11 @@
         <v>0.11990000000000001</v>
       </c>
       <c r="E21">
-        <f>AVERAGE(C21:D21)</f>
+        <f t="shared" si="0"/>
         <v>0.1237</v>
       </c>
       <c r="F21">
-        <f>980.61*E21+2.4087</f>
+        <f t="shared" si="1"/>
         <v>123.710157</v>
       </c>
     </row>
@@ -11851,11 +11855,11 @@
         <v>5.3999999999999999E-2</v>
       </c>
       <c r="E22">
-        <f>AVERAGE(C22:D22)</f>
+        <f t="shared" si="0"/>
         <v>5.6950000000000001E-2</v>
       </c>
       <c r="F22">
-        <f>980.61*E22+2.4087</f>
+        <f t="shared" si="1"/>
         <v>58.254439500000004</v>
       </c>
     </row>
@@ -11873,11 +11877,11 @@
         <v>7.3499999999999996E-2</v>
       </c>
       <c r="E23">
-        <f>AVERAGE(C23:D23)</f>
+        <f t="shared" si="0"/>
         <v>7.3399999999999993E-2</v>
       </c>
       <c r="F23">
-        <f>980.61*E23+2.4087</f>
+        <f t="shared" si="1"/>
         <v>74.385473999999988</v>
       </c>
     </row>
@@ -11895,11 +11899,11 @@
         <v>4.82E-2</v>
       </c>
       <c r="E24">
-        <f>AVERAGE(C24:D24)</f>
+        <f t="shared" si="0"/>
         <v>0.05</v>
       </c>
       <c r="F24">
-        <f>980.61*E24+2.4087</f>
+        <f t="shared" si="1"/>
         <v>51.439200000000007</v>
       </c>
     </row>
@@ -11917,11 +11921,11 @@
         <v>2.2800000000000001E-2</v>
       </c>
       <c r="E25">
-        <f>AVERAGE(C25:D25)</f>
+        <f t="shared" si="0"/>
         <v>2.2600000000000002E-2</v>
       </c>
       <c r="F25">
-        <f>980.61*E25+2.4087</f>
+        <f t="shared" si="1"/>
         <v>24.570486000000002</v>
       </c>
     </row>
@@ -11939,11 +11943,11 @@
         <v>6.3299999999999995E-2</v>
       </c>
       <c r="E26">
-        <f>AVERAGE(C26:D26)</f>
+        <f t="shared" si="0"/>
         <v>6.0149999999999995E-2</v>
       </c>
       <c r="F26">
-        <f>980.61*E26+2.4087</f>
+        <f t="shared" si="1"/>
         <v>61.392391500000002</v>
       </c>
     </row>
@@ -11961,11 +11965,11 @@
         <v>6.2100000000000002E-2</v>
       </c>
       <c r="E27">
-        <f>AVERAGE(C27:D27)</f>
+        <f t="shared" si="0"/>
         <v>6.2449999999999999E-2</v>
       </c>
       <c r="F27">
-        <f>980.61*E27+2.4087</f>
+        <f t="shared" si="1"/>
         <v>63.647794500000003</v>
       </c>
     </row>
@@ -11983,11 +11987,11 @@
         <v>2.5100000000000001E-2</v>
       </c>
       <c r="E28">
-        <f>AVERAGE(C28:D28)</f>
+        <f t="shared" si="0"/>
         <v>2.435E-2</v>
       </c>
       <c r="F28">
-        <f>980.61*E28+2.4087</f>
+        <f t="shared" si="1"/>
         <v>26.2865535</v>
       </c>
     </row>
@@ -12005,11 +12009,11 @@
         <v>3.73E-2</v>
       </c>
       <c r="E29">
-        <f>AVERAGE(C29:D29)</f>
+        <f t="shared" si="0"/>
         <v>3.09E-2</v>
       </c>
       <c r="F29">
-        <f>980.61*E29+2.4087</f>
+        <f t="shared" si="1"/>
         <v>32.709549000000003</v>
       </c>
     </row>
@@ -12027,11 +12031,11 @@
         <v>3.9199999999999999E-2</v>
       </c>
       <c r="E30">
-        <f>AVERAGE(C30:D30)</f>
+        <f t="shared" si="0"/>
         <v>4.3049999999999998E-2</v>
       </c>
       <c r="F30">
-        <f>980.61*E30+2.4087</f>
+        <f t="shared" si="1"/>
         <v>44.623960500000003</v>
       </c>
     </row>
@@ -12049,11 +12053,11 @@
         <v>4.1000000000000002E-2</v>
       </c>
       <c r="E31">
-        <f>AVERAGE(C31:D31)</f>
+        <f t="shared" si="0"/>
         <v>4.1450000000000001E-2</v>
       </c>
       <c r="F31">
-        <f>980.61*E31+2.4087</f>
+        <f t="shared" si="1"/>
         <v>43.054984500000003</v>
       </c>
     </row>
@@ -12071,11 +12075,11 @@
         <v>2.1499999999999998E-2</v>
       </c>
       <c r="E32">
-        <f>AVERAGE(C32:D32)</f>
+        <f t="shared" si="0"/>
         <v>2.1850000000000001E-2</v>
       </c>
       <c r="F32">
-        <f>980.61*E32+2.4087</f>
+        <f t="shared" si="1"/>
         <v>23.8350285</v>
       </c>
     </row>
@@ -12093,11 +12097,11 @@
         <v>1.5100000000000001E-2</v>
       </c>
       <c r="E33">
-        <f>AVERAGE(C33:D33)</f>
+        <f t="shared" si="0"/>
         <v>1.7649999999999999E-2</v>
       </c>
       <c r="F33">
-        <f>980.61*E33+2.4087</f>
+        <f t="shared" si="1"/>
         <v>19.716466499999999</v>
       </c>
     </row>
@@ -12115,11 +12119,11 @@
         <v>2.1700000000000001E-2</v>
       </c>
       <c r="E34">
-        <f>AVERAGE(C34:D34)</f>
+        <f t="shared" ref="E34:E65" si="2">AVERAGE(C34:D34)</f>
         <v>1.985E-2</v>
       </c>
       <c r="F34">
-        <f>980.61*E34+2.4087</f>
+        <f t="shared" ref="F34:F65" si="3">980.61*E34+2.4087</f>
         <v>21.873808499999999</v>
       </c>
     </row>
@@ -12137,11 +12141,11 @@
         <v>6</v>
       </c>
       <c r="E35" t="e">
-        <f>AVERAGE(C35:D35)</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="F35" t="e">
-        <f>980.61*E35+2.4087</f>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -12159,11 +12163,11 @@
         <v>1.78E-2</v>
       </c>
       <c r="E36">
-        <f>AVERAGE(C36:D36)</f>
+        <f t="shared" si="2"/>
         <v>1.8200000000000001E-2</v>
       </c>
       <c r="F36">
-        <f>980.61*E36+2.4087</f>
+        <f t="shared" si="3"/>
         <v>20.255801999999999</v>
       </c>
     </row>
@@ -12181,11 +12185,11 @@
         <v>2.0799999999999999E-2</v>
       </c>
       <c r="E37">
-        <f>AVERAGE(C37:D37)</f>
+        <f t="shared" si="2"/>
         <v>2.0499999999999997E-2</v>
       </c>
       <c r="F37">
-        <f>980.61*E37+2.4087</f>
+        <f t="shared" si="3"/>
         <v>22.511204999999997</v>
       </c>
     </row>
@@ -12203,11 +12207,11 @@
         <v>1.7999999999999999E-2</v>
       </c>
       <c r="E38">
-        <f>AVERAGE(C38:D38)</f>
+        <f t="shared" si="2"/>
         <v>2.095E-2</v>
       </c>
       <c r="F38">
-        <f>980.61*E38+2.4087</f>
+        <f t="shared" si="3"/>
         <v>22.952479499999999</v>
       </c>
     </row>
@@ -12225,11 +12229,11 @@
         <v>1.5599999999999999E-2</v>
       </c>
       <c r="E39">
-        <f>AVERAGE(C39:D39)</f>
+        <f t="shared" si="2"/>
         <v>1.6E-2</v>
       </c>
       <c r="F39">
-        <f>980.61*E39+2.4087</f>
+        <f t="shared" si="3"/>
         <v>18.098459999999999</v>
       </c>
     </row>
@@ -12247,11 +12251,11 @@
         <v>2.1600000000000001E-2</v>
       </c>
       <c r="E40">
-        <f>AVERAGE(C40:D40)</f>
+        <f t="shared" si="2"/>
         <v>2.0700000000000003E-2</v>
       </c>
       <c r="F40">
-        <f>980.61*E40+2.4087</f>
+        <f t="shared" si="3"/>
         <v>22.707327000000003</v>
       </c>
     </row>
@@ -12269,11 +12273,11 @@
         <v>2.0799999999999999E-2</v>
       </c>
       <c r="E41">
-        <f>AVERAGE(C41:D41)</f>
+        <f t="shared" si="2"/>
         <v>2.1499999999999998E-2</v>
       </c>
       <c r="F41">
-        <f>980.61*E41+2.4087</f>
+        <f t="shared" si="3"/>
         <v>23.491814999999999</v>
       </c>
     </row>
@@ -12291,11 +12295,11 @@
         <v>1.9599999999999999E-2</v>
       </c>
       <c r="E42">
-        <f>AVERAGE(C42:D42)</f>
+        <f t="shared" si="2"/>
         <v>1.7049999999999999E-2</v>
       </c>
       <c r="F42">
-        <f>980.61*E42+2.4087</f>
+        <f t="shared" si="3"/>
         <v>19.128100499999999</v>
       </c>
     </row>
@@ -12313,11 +12317,11 @@
         <v>3.3700000000000001E-2</v>
       </c>
       <c r="E43">
-        <f>AVERAGE(C43:D43)</f>
+        <f t="shared" si="2"/>
         <v>3.15E-2</v>
       </c>
       <c r="F43">
-        <f>980.61*E43+2.4087</f>
+        <f t="shared" si="3"/>
         <v>33.297915000000003</v>
       </c>
     </row>
@@ -12335,11 +12339,11 @@
         <v>1.67E-2</v>
       </c>
       <c r="E44">
-        <f>AVERAGE(C44:D44)</f>
+        <f t="shared" si="2"/>
         <v>1.6300000000000002E-2</v>
       </c>
       <c r="F44">
-        <f>980.61*E44+2.4087</f>
+        <f t="shared" si="3"/>
         <v>18.392643000000003</v>
       </c>
     </row>
@@ -12357,11 +12361,11 @@
         <v>1.89E-2</v>
       </c>
       <c r="E45">
-        <f>AVERAGE(C45:D45)</f>
+        <f t="shared" si="2"/>
         <v>1.7899999999999999E-2</v>
       </c>
       <c r="F45">
-        <f>980.61*E45+2.4087</f>
+        <f t="shared" si="3"/>
         <v>19.961618999999999</v>
       </c>
     </row>
@@ -12379,11 +12383,11 @@
         <v>1.6E-2</v>
       </c>
       <c r="E46">
-        <f>AVERAGE(C46:D46)</f>
+        <f t="shared" si="2"/>
         <v>1.78E-2</v>
       </c>
       <c r="F46">
-        <f>980.61*E46+2.4087</f>
+        <f t="shared" si="3"/>
         <v>19.863558000000001</v>
       </c>
     </row>
@@ -12401,11 +12405,11 @@
         <v>3.7900000000000003E-2</v>
       </c>
       <c r="E47">
-        <f>AVERAGE(C47:D47)</f>
+        <f t="shared" si="2"/>
         <v>3.9300000000000002E-2</v>
       </c>
       <c r="F47">
-        <f>980.61*E47+2.4087</f>
+        <f t="shared" si="3"/>
         <v>40.946673000000004</v>
       </c>
     </row>
@@ -12423,11 +12427,11 @@
         <v>4.4699999999999997E-2</v>
       </c>
       <c r="E48">
-        <f>AVERAGE(C48:D48)</f>
+        <f t="shared" si="2"/>
         <v>5.1049999999999998E-2</v>
       </c>
       <c r="F48">
-        <f>980.61*E48+2.4087</f>
+        <f t="shared" si="3"/>
         <v>52.468840499999999</v>
       </c>
     </row>
@@ -12445,11 +12449,11 @@
         <v>2.1299999999999999E-2</v>
       </c>
       <c r="E49">
-        <f>AVERAGE(C49:D49)</f>
+        <f t="shared" si="2"/>
         <v>2.0449999999999999E-2</v>
       </c>
       <c r="F49">
-        <f>980.61*E49+2.4087</f>
+        <f t="shared" si="3"/>
         <v>22.4621745</v>
       </c>
     </row>
@@ -12467,11 +12471,11 @@
         <v>1.9400000000000001E-2</v>
       </c>
       <c r="E50">
-        <f>AVERAGE(C50:D50)</f>
+        <f t="shared" si="2"/>
         <v>2.2600000000000002E-2</v>
       </c>
       <c r="F50">
-        <f>980.61*E50+2.4087</f>
+        <f t="shared" si="3"/>
         <v>24.570486000000002</v>
       </c>
     </row>
@@ -12489,11 +12493,11 @@
         <v>2.4E-2</v>
       </c>
       <c r="E51">
-        <f>AVERAGE(C51:D51)</f>
+        <f t="shared" si="2"/>
         <v>2.52E-2</v>
       </c>
       <c r="F51">
-        <f>980.61*E51+2.4087</f>
+        <f t="shared" si="3"/>
         <v>27.120072</v>
       </c>
     </row>
@@ -12511,11 +12515,11 @@
         <v>4.6600000000000003E-2</v>
       </c>
       <c r="E52">
-        <f>AVERAGE(C52:D52)</f>
+        <f t="shared" si="2"/>
         <v>4.7649999999999998E-2</v>
       </c>
       <c r="F52">
-        <f>980.61*E52+2.4087</f>
+        <f t="shared" si="3"/>
         <v>49.134766500000005</v>
       </c>
     </row>
@@ -12533,11 +12537,11 @@
         <v>0.05</v>
       </c>
       <c r="E53">
-        <f>AVERAGE(C53:D53)</f>
+        <f t="shared" si="2"/>
         <v>4.65E-2</v>
       </c>
       <c r="F53">
-        <f>980.61*E53+2.4087</f>
+        <f t="shared" si="3"/>
         <v>48.007065000000004</v>
       </c>
     </row>
@@ -12555,11 +12559,11 @@
         <v>5.6099999999999997E-2</v>
       </c>
       <c r="E54">
-        <f>AVERAGE(C54:D54)</f>
+        <f t="shared" si="2"/>
         <v>5.5999999999999994E-2</v>
       </c>
       <c r="F54">
-        <f>980.61*E54+2.4087</f>
+        <f t="shared" si="3"/>
         <v>57.322859999999999</v>
       </c>
     </row>
@@ -12577,11 +12581,11 @@
         <v>3.4799999999999998E-2</v>
       </c>
       <c r="E55">
-        <f>AVERAGE(C55:D55)</f>
+        <f t="shared" si="2"/>
         <v>3.32E-2</v>
       </c>
       <c r="F55">
-        <f>980.61*E55+2.4087</f>
+        <f t="shared" si="3"/>
         <v>34.964952000000004</v>
       </c>
     </row>
@@ -12599,11 +12603,11 @@
         <v>3.3599999999999998E-2</v>
       </c>
       <c r="E56">
-        <f>AVERAGE(C56:D56)</f>
+        <f t="shared" si="2"/>
         <v>3.1600000000000003E-2</v>
       </c>
       <c r="F56">
-        <f>980.61*E56+2.4087</f>
+        <f t="shared" si="3"/>
         <v>33.395976000000005</v>
       </c>
     </row>
@@ -12621,11 +12625,11 @@
         <v>2.6700000000000002E-2</v>
       </c>
       <c r="E57">
-        <f>AVERAGE(C57:D57)</f>
+        <f t="shared" si="2"/>
         <v>2.7450000000000002E-2</v>
       </c>
       <c r="F57">
-        <f>980.61*E57+2.4087</f>
+        <f t="shared" si="3"/>
         <v>29.326444500000001</v>
       </c>
     </row>
@@ -12643,11 +12647,11 @@
         <v>2.7400000000000001E-2</v>
       </c>
       <c r="E58">
-        <f>AVERAGE(C58:D58)</f>
+        <f t="shared" si="2"/>
         <v>2.86E-2</v>
       </c>
       <c r="F58">
-        <f>980.61*E58+2.4087</f>
+        <f t="shared" si="3"/>
         <v>30.454146000000001</v>
       </c>
     </row>
@@ -12665,11 +12669,11 @@
         <v>1.2E-2</v>
       </c>
       <c r="E59">
-        <f>AVERAGE(C59:D59)</f>
+        <f t="shared" si="2"/>
         <v>9.4000000000000004E-3</v>
       </c>
       <c r="F59">
-        <f>980.61*E59+2.4087</f>
+        <f t="shared" si="3"/>
         <v>11.626434</v>
       </c>
     </row>
@@ -12687,11 +12691,11 @@
         <v>4.4699999999999997E-2</v>
       </c>
       <c r="E60">
-        <f>AVERAGE(C60:D60)</f>
+        <f t="shared" si="2"/>
         <v>4.3749999999999997E-2</v>
       </c>
       <c r="F60">
-        <f>980.61*E60+2.4087</f>
+        <f t="shared" si="3"/>
         <v>45.310387500000004</v>
       </c>
     </row>
@@ -12709,11 +12713,11 @@
         <v>3.5999999999999997E-2</v>
       </c>
       <c r="E61">
-        <f>AVERAGE(C61:D61)</f>
+        <f t="shared" si="2"/>
         <v>3.5749999999999997E-2</v>
       </c>
       <c r="F61">
-        <f>980.61*E61+2.4087</f>
+        <f t="shared" si="3"/>
         <v>37.465507500000001</v>
       </c>
     </row>
@@ -12731,11 +12735,11 @@
         <v>2.4199999999999999E-2</v>
       </c>
       <c r="E62">
-        <f>AVERAGE(C62:D62)</f>
+        <f t="shared" si="2"/>
         <v>2.3949999999999999E-2</v>
       </c>
       <c r="F62">
-        <f>980.61*E62+2.4087</f>
+        <f t="shared" si="3"/>
         <v>25.894309499999999</v>
       </c>
     </row>
@@ -12753,11 +12757,11 @@
         <v>1.55E-2</v>
       </c>
       <c r="E63">
-        <f>AVERAGE(C63:D63)</f>
+        <f t="shared" si="2"/>
         <v>1.6050000000000002E-2</v>
       </c>
       <c r="F63">
-        <f>980.61*E63+2.4087</f>
+        <f t="shared" si="3"/>
         <v>18.147490500000004</v>
       </c>
     </row>
@@ -12775,11 +12779,11 @@
         <v>2.3199999999999998E-2</v>
       </c>
       <c r="E64">
-        <f>AVERAGE(C64:D64)</f>
+        <f t="shared" si="2"/>
         <v>1.9999999999999997E-2</v>
       </c>
       <c r="F64">
-        <f>980.61*E64+2.4087</f>
+        <f t="shared" si="3"/>
         <v>22.020899999999997</v>
       </c>
     </row>
@@ -12797,11 +12801,11 @@
         <v>3.3399999999999999E-2</v>
       </c>
       <c r="E65">
-        <f>AVERAGE(C65:D65)</f>
+        <f t="shared" si="2"/>
         <v>3.1600000000000003E-2</v>
       </c>
       <c r="F65">
-        <f>980.61*E65+2.4087</f>
+        <f t="shared" si="3"/>
         <v>33.395976000000005</v>
       </c>
     </row>
@@ -12819,11 +12823,11 @@
         <v>5.2900000000000003E-2</v>
       </c>
       <c r="E66">
-        <f>AVERAGE(C66:D66)</f>
+        <f t="shared" ref="E66:E97" si="4">AVERAGE(C66:D66)</f>
         <v>5.3650000000000003E-2</v>
       </c>
       <c r="F66">
-        <f>980.61*E66+2.4087</f>
+        <f t="shared" ref="F66:F97" si="5">980.61*E66+2.4087</f>
         <v>55.018426500000004</v>
       </c>
     </row>
@@ -12841,11 +12845,11 @@
         <v>3.9800000000000002E-2</v>
       </c>
       <c r="E67">
-        <f>AVERAGE(C67:D67)</f>
+        <f t="shared" si="4"/>
         <v>4.5450000000000004E-2</v>
       </c>
       <c r="F67">
-        <f>980.61*E67+2.4087</f>
+        <f t="shared" si="5"/>
         <v>46.977424500000005</v>
       </c>
     </row>
@@ -12863,11 +12867,11 @@
         <v>1.54E-2</v>
       </c>
       <c r="E68">
-        <f>AVERAGE(C68:D68)</f>
+        <f t="shared" si="4"/>
         <v>1.745E-2</v>
       </c>
       <c r="F68">
-        <f>980.61*E68+2.4087</f>
+        <f t="shared" si="5"/>
         <v>19.5203445</v>
       </c>
     </row>
@@ -12885,11 +12889,11 @@
         <v>0.45219999999999999</v>
       </c>
       <c r="E69">
-        <f>AVERAGE(C69:D69)</f>
+        <f t="shared" si="4"/>
         <v>0.44059999999999999</v>
       </c>
       <c r="F69">
-        <f>980.61*E69+2.4087</f>
+        <f t="shared" si="5"/>
         <v>434.46546599999999</v>
       </c>
     </row>
@@ -12907,11 +12911,11 @@
         <v>0.20100000000000001</v>
       </c>
       <c r="E70">
-        <f>AVERAGE(C70:D70)</f>
+        <f t="shared" si="4"/>
         <v>0.1978</v>
       </c>
       <c r="F70">
-        <f>980.61*E70+2.4087</f>
+        <f t="shared" si="5"/>
         <v>196.37335800000002</v>
       </c>
     </row>
@@ -12929,11 +12933,11 @@
         <v>0.28220000000000001</v>
       </c>
       <c r="E71">
-        <f>AVERAGE(C71:D71)</f>
+        <f t="shared" si="4"/>
         <v>0.28444999999999998</v>
       </c>
       <c r="F71">
-        <f>980.61*E71+2.4087</f>
+        <f t="shared" si="5"/>
         <v>281.34321449999999</v>
       </c>
     </row>
@@ -12951,11 +12955,11 @@
         <v>0.2223</v>
       </c>
       <c r="E72">
-        <f>AVERAGE(C72:D72)</f>
+        <f t="shared" si="4"/>
         <v>0.21829999999999999</v>
       </c>
       <c r="F72">
-        <f>980.61*E72+2.4087</f>
+        <f t="shared" si="5"/>
         <v>216.475863</v>
       </c>
     </row>
@@ -12973,11 +12977,11 @@
         <v>8.9599999999999999E-2</v>
       </c>
       <c r="E73">
-        <f>AVERAGE(C73:D73)</f>
+        <f t="shared" si="4"/>
         <v>9.0700000000000003E-2</v>
       </c>
       <c r="F73">
-        <f>980.61*E73+2.4087</f>
+        <f t="shared" si="5"/>
         <v>91.350026999999997</v>
       </c>
     </row>
@@ -12995,11 +12999,11 @@
         <v>0.2661</v>
       </c>
       <c r="E74">
-        <f>AVERAGE(C74:D74)</f>
+        <f t="shared" si="4"/>
         <v>0.27044999999999997</v>
       </c>
       <c r="F74">
-        <f>980.61*E74+2.4087</f>
+        <f t="shared" si="5"/>
         <v>267.61467449999998</v>
       </c>
     </row>
@@ -13017,11 +13021,11 @@
         <v>0.29780000000000001</v>
       </c>
       <c r="E75">
-        <f>AVERAGE(C75:D75)</f>
+        <f t="shared" si="4"/>
         <v>0.29744999999999999</v>
       </c>
       <c r="F75">
-        <f>980.61*E75+2.4087</f>
+        <f t="shared" si="5"/>
         <v>294.09114449999998</v>
       </c>
     </row>
@@ -13039,11 +13043,11 @@
         <v>0.4037</v>
       </c>
       <c r="E76">
-        <f>AVERAGE(C76:D76)</f>
+        <f t="shared" si="4"/>
         <v>0.41425000000000001</v>
       </c>
       <c r="F76">
-        <f>980.61*E76+2.4087</f>
+        <f t="shared" si="5"/>
         <v>408.62639250000001</v>
       </c>
     </row>
@@ -13061,11 +13065,11 @@
         <v>0.24610000000000001</v>
       </c>
       <c r="E77">
-        <f>AVERAGE(C77:D77)</f>
+        <f t="shared" si="4"/>
         <v>0.24175000000000002</v>
       </c>
       <c r="F77">
-        <f>980.61*E77+2.4087</f>
+        <f t="shared" si="5"/>
         <v>239.47116750000004</v>
       </c>
     </row>
@@ -13083,11 +13087,11 @@
         <v>0.18440000000000001</v>
       </c>
       <c r="E78">
-        <f>AVERAGE(C78:D78)</f>
+        <f t="shared" si="4"/>
         <v>0.18814999999999998</v>
       </c>
       <c r="F78">
-        <f>980.61*E78+2.4087</f>
+        <f t="shared" si="5"/>
         <v>186.9104715</v>
       </c>
     </row>
@@ -13105,11 +13109,11 @@
         <v>0.17269999999999999</v>
       </c>
       <c r="E79">
-        <f>AVERAGE(C79:D79)</f>
+        <f t="shared" si="4"/>
         <v>0.1716</v>
       </c>
       <c r="F79">
-        <f>980.61*E79+2.4087</f>
+        <f t="shared" si="5"/>
         <v>170.68137600000003</v>
       </c>
     </row>
@@ -13127,11 +13131,11 @@
         <v>0.2281</v>
       </c>
       <c r="E80">
-        <f>AVERAGE(C80:D80)</f>
+        <f t="shared" si="4"/>
         <v>0.22409999999999999</v>
       </c>
       <c r="F80">
-        <f>980.61*E80+2.4087</f>
+        <f t="shared" si="5"/>
         <v>222.16340099999999</v>
       </c>
     </row>
@@ -13149,11 +13153,11 @@
         <v>0.26900000000000002</v>
       </c>
       <c r="E81">
-        <f>AVERAGE(C81:D81)</f>
+        <f t="shared" si="4"/>
         <v>0.26965</v>
       </c>
       <c r="F81">
-        <f>980.61*E81+2.4087</f>
+        <f t="shared" si="5"/>
         <v>266.83018650000002</v>
       </c>
     </row>
@@ -13171,11 +13175,11 @@
         <v>0.26479999999999998</v>
       </c>
       <c r="E82">
-        <f>AVERAGE(C82:D82)</f>
+        <f t="shared" si="4"/>
         <v>0.26300000000000001</v>
       </c>
       <c r="F82">
-        <f>980.61*E82+2.4087</f>
+        <f t="shared" si="5"/>
         <v>260.30913000000004</v>
       </c>
     </row>
@@ -13193,11 +13197,11 @@
         <v>0.21460000000000001</v>
       </c>
       <c r="E83">
-        <f>AVERAGE(C83:D83)</f>
+        <f t="shared" si="4"/>
         <v>0.27315</v>
       </c>
       <c r="F83">
-        <f>980.61*E83+2.4087</f>
+        <f t="shared" si="5"/>
         <v>270.26232150000004</v>
       </c>
     </row>
@@ -13215,11 +13219,11 @@
         <v>0.33839999999999998</v>
       </c>
       <c r="E84">
-        <f>AVERAGE(C84:D84)</f>
+        <f t="shared" si="4"/>
         <v>0.28320000000000001</v>
       </c>
       <c r="F84">
-        <f>980.61*E84+2.4087</f>
+        <f t="shared" si="5"/>
         <v>280.11745200000001</v>
       </c>
     </row>
@@ -13237,11 +13241,11 @@
         <v>0.30919999999999997</v>
       </c>
       <c r="E85">
-        <f>AVERAGE(C85:D85)</f>
+        <f t="shared" si="4"/>
         <v>0.30754999999999999</v>
       </c>
       <c r="F85">
-        <f>980.61*E85+2.4087</f>
+        <f t="shared" si="5"/>
         <v>303.99530550000003</v>
       </c>
     </row>
@@ -13259,11 +13263,11 @@
         <v>0.1696</v>
       </c>
       <c r="E86">
-        <f>AVERAGE(C86:D86)</f>
+        <f t="shared" si="4"/>
         <v>0.1658</v>
       </c>
       <c r="F86">
-        <f>980.61*E86+2.4087</f>
+        <f t="shared" si="5"/>
         <v>164.99383800000001</v>
       </c>
     </row>
@@ -13281,11 +13285,11 @@
         <v>0.16420000000000001</v>
       </c>
       <c r="E87">
-        <f>AVERAGE(C87:D87)</f>
+        <f t="shared" si="4"/>
         <v>0.16470000000000001</v>
       </c>
       <c r="F87">
-        <f>980.61*E87+2.4087</f>
+        <f t="shared" si="5"/>
         <v>163.91516700000003</v>
       </c>
     </row>
@@ -13303,11 +13307,11 @@
         <v>2.6599999999999999E-2</v>
       </c>
       <c r="E88">
-        <f>AVERAGE(C88:D88)</f>
+        <f t="shared" si="4"/>
         <v>2.8999999999999998E-2</v>
       </c>
       <c r="F88">
-        <f>980.61*E88+2.4087</f>
+        <f t="shared" si="5"/>
         <v>30.84639</v>
       </c>
     </row>
@@ -13325,11 +13329,11 @@
         <v>7.8700000000000006E-2</v>
       </c>
       <c r="E89">
-        <f>AVERAGE(C89:D89)</f>
+        <f t="shared" si="4"/>
         <v>8.1500000000000003E-2</v>
       </c>
       <c r="F89">
-        <f>980.61*E89+2.4087</f>
+        <f t="shared" si="5"/>
         <v>82.328415000000007</v>
       </c>
     </row>
@@ -13347,11 +13351,11 @@
         <v>5.8200000000000002E-2</v>
       </c>
       <c r="E90">
-        <f>AVERAGE(C90:D90)</f>
+        <f t="shared" si="4"/>
         <v>5.7749999999999996E-2</v>
       </c>
       <c r="F90">
-        <f>980.61*E90+2.4087</f>
+        <f t="shared" si="5"/>
         <v>59.0389275</v>
       </c>
     </row>
@@ -13369,11 +13373,11 @@
         <v>9.2299999999999993E-2</v>
       </c>
       <c r="E91">
-        <f>AVERAGE(C91:D91)</f>
+        <f t="shared" si="4"/>
         <v>9.1700000000000004E-2</v>
       </c>
       <c r="F91">
-        <f>980.61*E91+2.4087</f>
+        <f t="shared" si="5"/>
         <v>92.330636999999996</v>
       </c>
     </row>
@@ -13391,11 +13395,11 @@
         <v>2.9100000000000001E-2</v>
       </c>
       <c r="E92">
-        <f>AVERAGE(C92:D92)</f>
+        <f t="shared" si="4"/>
         <v>2.93E-2</v>
       </c>
       <c r="F92">
-        <f>980.61*E92+2.4087</f>
+        <f t="shared" si="5"/>
         <v>31.140573</v>
       </c>
     </row>
@@ -13413,11 +13417,11 @@
         <v>0.45369999999999999</v>
       </c>
       <c r="E93">
-        <f>AVERAGE(C93:D93)</f>
+        <f t="shared" si="4"/>
         <v>0.45405000000000001</v>
       </c>
       <c r="F93">
-        <f>980.61*E93+2.4087</f>
+        <f t="shared" si="5"/>
         <v>447.65467050000001</v>
       </c>
     </row>
@@ -13435,11 +13439,11 @@
         <v>3.0300000000000001E-2</v>
       </c>
       <c r="E94">
-        <f>AVERAGE(C94:D94)</f>
+        <f t="shared" si="4"/>
         <v>2.8400000000000002E-2</v>
       </c>
       <c r="F94">
-        <f>980.61*E94+2.4087</f>
+        <f t="shared" si="5"/>
         <v>30.258024000000002</v>
       </c>
     </row>
@@ -13457,11 +13461,11 @@
         <v>0.13900000000000001</v>
       </c>
       <c r="E95">
-        <f>AVERAGE(C95:D95)</f>
+        <f t="shared" si="4"/>
         <v>0.14005000000000001</v>
       </c>
       <c r="F95">
-        <f>980.61*E95+2.4087</f>
+        <f t="shared" si="5"/>
         <v>139.74313050000001</v>
       </c>
     </row>
@@ -13479,11 +13483,11 @@
         <v>6.2700000000000006E-2</v>
       </c>
       <c r="E96">
-        <f>AVERAGE(C96:D96)</f>
+        <f t="shared" si="4"/>
         <v>6.4049999999999996E-2</v>
       </c>
       <c r="F96">
-        <f>980.61*E96+2.4087</f>
+        <f t="shared" si="5"/>
         <v>65.216770499999996</v>
       </c>
     </row>
@@ -13501,11 +13505,11 @@
         <v>7.9000000000000001E-2</v>
       </c>
       <c r="E97">
-        <f>AVERAGE(C97:D97)</f>
+        <f t="shared" si="4"/>
         <v>7.3800000000000004E-2</v>
       </c>
       <c r="F97">
-        <f>980.61*E97+2.4087</f>
+        <f t="shared" si="5"/>
         <v>74.777718000000007</v>
       </c>
     </row>
@@ -13523,11 +13527,11 @@
         <v>0.1196</v>
       </c>
       <c r="E98">
-        <f>AVERAGE(C98:D98)</f>
+        <f t="shared" ref="E98:E129" si="6">AVERAGE(C98:D98)</f>
         <v>0.1148</v>
       </c>
       <c r="F98">
-        <f>980.61*E98+2.4087</f>
+        <f t="shared" ref="F98:F129" si="7">980.61*E98+2.4087</f>
         <v>114.98272799999999</v>
       </c>
     </row>
@@ -13545,11 +13549,11 @@
         <v>3.4000000000000002E-2</v>
       </c>
       <c r="E99">
-        <f>AVERAGE(C99:D99)</f>
+        <f t="shared" si="6"/>
         <v>2.98E-2</v>
       </c>
       <c r="F99">
-        <f>980.61*E99+2.4087</f>
+        <f t="shared" si="7"/>
         <v>31.630877999999999</v>
       </c>
     </row>
@@ -13567,11 +13571,11 @@
         <v>0.15820000000000001</v>
       </c>
       <c r="E100">
-        <f>AVERAGE(C100:D100)</f>
+        <f t="shared" si="6"/>
         <v>0.15579999999999999</v>
       </c>
       <c r="F100">
-        <f>980.61*E100+2.4087</f>
+        <f t="shared" si="7"/>
         <v>155.187738</v>
       </c>
     </row>
@@ -13589,11 +13593,11 @@
         <v>4.0599999999999997E-2</v>
       </c>
       <c r="E101">
-        <f>AVERAGE(C101:D101)</f>
+        <f t="shared" si="6"/>
         <v>3.9199999999999999E-2</v>
       </c>
       <c r="F101">
-        <f>980.61*E101+2.4087</f>
+        <f t="shared" si="7"/>
         <v>40.848612000000003</v>
       </c>
     </row>
@@ -13611,11 +13615,11 @@
         <v>4.5499999999999999E-2</v>
       </c>
       <c r="E102">
-        <f>AVERAGE(C102:D102)</f>
+        <f t="shared" si="6"/>
         <v>3.8599999999999995E-2</v>
       </c>
       <c r="F102">
-        <f>980.61*E102+2.4087</f>
+        <f t="shared" si="7"/>
         <v>40.260246000000002</v>
       </c>
     </row>
@@ -13633,11 +13637,11 @@
         <v>2.7799999999999998E-2</v>
       </c>
       <c r="E103">
-        <f>AVERAGE(C103:D103)</f>
+        <f t="shared" si="6"/>
         <v>3.0799999999999998E-2</v>
       </c>
       <c r="F103">
-        <f>980.61*E103+2.4087</f>
+        <f t="shared" si="7"/>
         <v>32.611488000000001</v>
       </c>
     </row>
@@ -13655,11 +13659,11 @@
         <v>8.3599999999999994E-2</v>
       </c>
       <c r="E104">
-        <f>AVERAGE(C104:D104)</f>
+        <f t="shared" si="6"/>
         <v>8.6849999999999997E-2</v>
       </c>
       <c r="F104">
-        <f>980.61*E104+2.4087</f>
+        <f t="shared" si="7"/>
         <v>87.57467849999999</v>
       </c>
     </row>
@@ -13677,11 +13681,11 @@
         <v>3.2500000000000001E-2</v>
       </c>
       <c r="E105">
-        <f>AVERAGE(C105:D105)</f>
+        <f t="shared" si="6"/>
         <v>3.2600000000000004E-2</v>
       </c>
       <c r="F105">
-        <f>980.61*E105+2.4087</f>
+        <f t="shared" si="7"/>
         <v>34.376586000000003</v>
       </c>
     </row>
@@ -13699,11 +13703,11 @@
         <v>2.4899999999999999E-2</v>
       </c>
       <c r="E106">
-        <f>AVERAGE(C106:D106)</f>
+        <f t="shared" si="6"/>
         <v>2.2350000000000002E-2</v>
       </c>
       <c r="F106">
-        <f>980.61*E106+2.4087</f>
+        <f t="shared" si="7"/>
         <v>24.325333500000003</v>
       </c>
     </row>
@@ -13721,11 +13725,11 @@
         <v>2.5700000000000001E-2</v>
       </c>
       <c r="E107">
-        <f>AVERAGE(C107:D107)</f>
+        <f t="shared" si="6"/>
         <v>2.3449999999999999E-2</v>
       </c>
       <c r="F107">
-        <f>980.61*E107+2.4087</f>
+        <f t="shared" si="7"/>
         <v>25.404004499999999</v>
       </c>
     </row>
@@ -13743,11 +13747,11 @@
         <v>2.3099999999999999E-2</v>
       </c>
       <c r="E108">
-        <f>AVERAGE(C108:D108)</f>
+        <f t="shared" si="6"/>
         <v>2.325E-2</v>
       </c>
       <c r="F108">
-        <f>980.61*E108+2.4087</f>
+        <f t="shared" si="7"/>
         <v>25.2078825</v>
       </c>
     </row>
@@ -13765,11 +13769,11 @@
         <v>6.8999999999999999E-3</v>
       </c>
       <c r="E109">
-        <f>AVERAGE(C109:D109)</f>
+        <f t="shared" si="6"/>
         <v>6.8999999999999999E-3</v>
       </c>
       <c r="F109">
-        <f>980.61*E109+2.4087</f>
+        <f t="shared" si="7"/>
         <v>9.1749089999999995</v>
       </c>
     </row>
@@ -13787,11 +13791,11 @@
         <v>1.12E-2</v>
       </c>
       <c r="E110">
-        <f>AVERAGE(C110:D110)</f>
+        <f t="shared" si="6"/>
         <v>1.065E-2</v>
       </c>
       <c r="F110">
-        <f>980.61*E110+2.4087</f>
+        <f t="shared" si="7"/>
         <v>12.8521965</v>
       </c>
     </row>
@@ -13809,11 +13813,11 @@
         <v>1.6799999999999999E-2</v>
       </c>
       <c r="E111">
-        <f>AVERAGE(C111:D111)</f>
+        <f t="shared" si="6"/>
         <v>1.345E-2</v>
       </c>
       <c r="F111">
-        <f>980.61*E111+2.4087</f>
+        <f t="shared" si="7"/>
         <v>15.5979045</v>
       </c>
     </row>
@@ -13831,11 +13835,11 @@
         <v>1.0200000000000001E-2</v>
       </c>
       <c r="E112">
-        <f>AVERAGE(C112:D112)</f>
+        <f t="shared" si="6"/>
         <v>1.005E-2</v>
       </c>
       <c r="F112">
-        <f>980.61*E112+2.4087</f>
+        <f t="shared" si="7"/>
         <v>12.263830499999999</v>
       </c>
     </row>
@@ -13853,11 +13857,11 @@
         <v>1.03E-2</v>
       </c>
       <c r="E113">
-        <f>AVERAGE(C113:D113)</f>
+        <f t="shared" si="6"/>
         <v>1.115E-2</v>
       </c>
       <c r="F113">
-        <f>980.61*E113+2.4087</f>
+        <f t="shared" si="7"/>
         <v>13.342501499999999</v>
       </c>
     </row>
@@ -13875,11 +13879,11 @@
         <v>0.01</v>
       </c>
       <c r="E114">
-        <f>AVERAGE(C114:D114)</f>
+        <f t="shared" si="6"/>
         <v>8.8999999999999999E-3</v>
       </c>
       <c r="F114">
-        <f>980.61*E114+2.4087</f>
+        <f t="shared" si="7"/>
         <v>11.136129</v>
       </c>
     </row>
@@ -14670,9 +14674,9 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1838D717-F380-49AF-B1BA-03E3C1FE5466}">
-  <dimension ref="A1:G116"/>
+  <dimension ref="A1:I116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
       <selection activeCell="I67" sqref="I67"/>
     </sheetView>
   </sheetViews>
@@ -14715,7 +14719,7 @@
         <v>0.27700000000000002</v>
       </c>
       <c r="E2">
-        <f>AVERAGE(C2:D2)</f>
+        <f t="shared" ref="E2:E33" si="0">AVERAGE(C2:D2)</f>
         <v>0.3095</v>
       </c>
       <c r="F2">
@@ -14741,7 +14745,7 @@
         <v>0.53100000000000003</v>
       </c>
       <c r="E3">
-        <f>AVERAGE(C3:D3)</f>
+        <f t="shared" si="0"/>
         <v>0.48350000000000004</v>
       </c>
       <c r="F3">
@@ -14749,7 +14753,7 @@
         <v>74.28146000000001</v>
       </c>
       <c r="G3">
-        <f t="shared" ref="G3:G66" si="0">F3*2</f>
+        <f t="shared" ref="G3:G66" si="1">F3*2</f>
         <v>148.56292000000002</v>
       </c>
     </row>
@@ -14767,7 +14771,7 @@
         <v>0.252</v>
       </c>
       <c r="E4">
-        <f>AVERAGE(C4:D4)</f>
+        <f t="shared" si="0"/>
         <v>0.29200000000000004</v>
       </c>
       <c r="F4">
@@ -14775,7 +14779,7 @@
         <v>52.175620000000009</v>
       </c>
       <c r="G4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>104.35124000000002</v>
       </c>
     </row>
@@ -14793,7 +14797,7 @@
         <v>0.51</v>
       </c>
       <c r="E5">
-        <f>AVERAGE(C5:D5)</f>
+        <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
       <c r="F5">
@@ -14801,7 +14805,7 @@
         <v>96.336100000000002</v>
       </c>
       <c r="G5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>192.6722</v>
       </c>
     </row>
@@ -14819,7 +14823,7 @@
         <v>0.28899999999999998</v>
       </c>
       <c r="E6">
-        <f>AVERAGE(C6:D6)</f>
+        <f t="shared" si="0"/>
         <v>0.29749999999999999</v>
       </c>
       <c r="F6">
@@ -14827,7 +14831,7 @@
         <v>53.343325</v>
       </c>
       <c r="G6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>106.68665</v>
       </c>
     </row>
@@ -14845,7 +14849,7 @@
         <v>0.53200000000000003</v>
       </c>
       <c r="E7">
-        <f>AVERAGE(C7:D7)</f>
+        <f t="shared" si="0"/>
         <v>0.65200000000000002</v>
       </c>
       <c r="F7">
@@ -14853,7 +14857,7 @@
         <v>104.73952</v>
       </c>
       <c r="G7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>209.47904</v>
       </c>
     </row>
@@ -14871,7 +14875,7 @@
         <v>0.13200000000000001</v>
       </c>
       <c r="E8">
-        <f>AVERAGE(C8:D8)</f>
+        <f t="shared" si="0"/>
         <v>0.129</v>
       </c>
       <c r="F8">
@@ -14879,7 +14883,7 @@
         <v>31.767150000000001</v>
       </c>
       <c r="G8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>63.534300000000002</v>
       </c>
     </row>
@@ -14897,7 +14901,7 @@
         <v>0.312</v>
       </c>
       <c r="E9">
-        <f>AVERAGE(C9:D9)</f>
+        <f t="shared" si="0"/>
         <v>0.314</v>
       </c>
       <c r="F9">
@@ -14905,7 +14909,7 @@
         <v>58.115380000000002</v>
       </c>
       <c r="G9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>116.23076</v>
       </c>
     </row>
@@ -14923,7 +14927,7 @@
         <v>0.19</v>
       </c>
       <c r="E10">
-        <f>AVERAGE(C10:D10)</f>
+        <f t="shared" si="0"/>
         <v>0.17799999999999999</v>
       </c>
       <c r="F10">
@@ -14931,7 +14935,7 @@
         <v>31.837459999999993</v>
       </c>
       <c r="G10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>63.674919999999986</v>
       </c>
     </row>
@@ -14949,7 +14953,7 @@
         <v>0.38200000000000001</v>
       </c>
       <c r="E11">
-        <f>AVERAGE(C11:D11)</f>
+        <f t="shared" si="0"/>
         <v>0.38850000000000001</v>
       </c>
       <c r="F11">
@@ -14957,7 +14961,7 @@
         <v>57.109259999999992</v>
       </c>
       <c r="G11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>114.21851999999998</v>
       </c>
     </row>
@@ -14975,7 +14979,7 @@
         <v>0.14299999999999999</v>
       </c>
       <c r="E12">
-        <f>AVERAGE(C12:D12)</f>
+        <f t="shared" si="0"/>
         <v>0.14299999999999999</v>
       </c>
       <c r="F12">
@@ -14983,7 +14987,7 @@
         <v>35.288849999999996</v>
       </c>
       <c r="G12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>70.577699999999993</v>
       </c>
     </row>
@@ -15001,7 +15005,7 @@
         <v>0.20100000000000001</v>
       </c>
       <c r="E13">
-        <f>AVERAGE(C13:D13)</f>
+        <f t="shared" si="0"/>
         <v>0.18</v>
       </c>
       <c r="F13">
@@ -15009,7 +15013,7 @@
         <v>44.596200000000003</v>
       </c>
       <c r="G13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>89.192400000000006</v>
       </c>
     </row>
@@ -15027,7 +15031,7 @@
         <v>0.20599999999999999</v>
       </c>
       <c r="E14">
-        <f>AVERAGE(C14:D14)</f>
+        <f t="shared" si="0"/>
         <v>0.21149999999999999</v>
       </c>
       <c r="F14">
@@ -15035,7 +15039,7 @@
         <v>38.310329999999993</v>
       </c>
       <c r="G14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>76.620659999999987</v>
       </c>
     </row>
@@ -15053,7 +15057,7 @@
         <v>0.28199999999999997</v>
       </c>
       <c r="E15">
-        <f>AVERAGE(C15:D15)</f>
+        <f t="shared" si="0"/>
         <v>0.28000000000000003</v>
       </c>
       <c r="F15">
@@ -15061,7 +15065,7 @@
         <v>51.545900000000003</v>
       </c>
       <c r="G15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>103.09180000000001</v>
       </c>
     </row>
@@ -15079,7 +15083,7 @@
         <v>0.41799999999999998</v>
       </c>
       <c r="E16">
-        <f>AVERAGE(C16:D16)</f>
+        <f t="shared" si="0"/>
         <v>0.41149999999999998</v>
       </c>
       <c r="F16">
@@ -15087,7 +15091,7 @@
         <v>102.83002499999999</v>
       </c>
       <c r="G16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>205.66004999999998</v>
       </c>
     </row>
@@ -15105,7 +15109,7 @@
         <v>0.19</v>
       </c>
       <c r="E17">
-        <f>AVERAGE(C17:D17)</f>
+        <f t="shared" si="0"/>
         <v>0.17849999999999999</v>
       </c>
       <c r="F17">
@@ -15113,7 +15117,7 @@
         <v>44.218874999999997</v>
       </c>
       <c r="G17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>88.437749999999994</v>
       </c>
     </row>
@@ -15131,7 +15135,7 @@
         <v>0.26800000000000002</v>
       </c>
       <c r="E18">
-        <f>AVERAGE(C18:D18)</f>
+        <f t="shared" si="0"/>
         <v>0.24299999999999999</v>
       </c>
       <c r="F18">
@@ -15139,7 +15143,7 @@
         <v>44.396759999999993</v>
       </c>
       <c r="G18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>88.793519999999987</v>
       </c>
     </row>
@@ -15157,7 +15161,7 @@
         <v>0.4</v>
       </c>
       <c r="E19">
-        <f>AVERAGE(C19:D19)</f>
+        <f t="shared" si="0"/>
         <v>0.36250000000000004</v>
       </c>
       <c r="F19">
@@ -15165,7 +15169,7 @@
         <v>90.504075000000014</v>
       </c>
       <c r="G19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>181.00815000000003</v>
       </c>
     </row>
@@ -15183,7 +15187,7 @@
         <v>9.1999999999999998E-2</v>
       </c>
       <c r="E20">
-        <f>AVERAGE(C20:D20)</f>
+        <f t="shared" si="0"/>
         <v>8.9499999999999996E-2</v>
       </c>
       <c r="F20">
@@ -15191,7 +15195,7 @@
         <v>21.830925000000001</v>
       </c>
       <c r="G20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>43.661850000000001</v>
       </c>
     </row>
@@ -15209,7 +15213,7 @@
         <v>1.9330000000000001</v>
       </c>
       <c r="E21">
-        <f>AVERAGE(C21:D21)</f>
+        <f t="shared" si="0"/>
         <v>1.831</v>
       </c>
       <c r="F21">
@@ -15217,7 +15221,7 @@
         <v>378.92070999999999</v>
       </c>
       <c r="G21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>757.84141999999997</v>
       </c>
     </row>
@@ -15235,7 +15239,7 @@
         <v>1.5840000000000001</v>
       </c>
       <c r="E22">
-        <f>AVERAGE(C22:D22)</f>
+        <f t="shared" si="0"/>
         <v>1.3725000000000001</v>
       </c>
       <c r="F22">
@@ -15243,7 +15247,7 @@
         <v>234.97710000000001</v>
       </c>
       <c r="G22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>469.95420000000001</v>
       </c>
     </row>
@@ -15261,7 +15265,7 @@
         <v>0.747</v>
       </c>
       <c r="E23">
-        <f>AVERAGE(C23:D23)</f>
+        <f t="shared" si="0"/>
         <v>0.76500000000000001</v>
       </c>
       <c r="F23">
@@ -15269,7 +15273,7 @@
         <v>145.2576</v>
       </c>
       <c r="G23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>290.51519999999999</v>
       </c>
     </row>
@@ -15287,7 +15291,7 @@
         <v>0.71099999999999997</v>
       </c>
       <c r="E24">
-        <f>AVERAGE(C24:D24)</f>
+        <f t="shared" si="0"/>
         <v>0.72449999999999992</v>
       </c>
       <c r="F24">
@@ -15295,7 +15299,7 @@
         <v>143.99969499999997</v>
       </c>
       <c r="G24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>287.99938999999995</v>
       </c>
     </row>
@@ -15313,7 +15317,7 @@
         <v>0.96199999999999997</v>
       </c>
       <c r="E25">
-        <f>AVERAGE(C25:D25)</f>
+        <f t="shared" si="0"/>
         <v>0.95150000000000001</v>
       </c>
       <c r="F25">
@@ -15321,7 +15325,7 @@
         <v>192.19406500000002</v>
       </c>
       <c r="G25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>384.38813000000005</v>
       </c>
     </row>
@@ -15339,7 +15343,7 @@
         <v>0.84599999999999997</v>
       </c>
       <c r="E26">
-        <f>AVERAGE(C26:D26)</f>
+        <f t="shared" si="0"/>
         <v>0.77149999999999996</v>
       </c>
       <c r="F26">
@@ -15347,7 +15351,7 @@
         <v>126.34033999999998</v>
       </c>
       <c r="G26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>252.68067999999997</v>
       </c>
     </row>
@@ -15365,7 +15369,7 @@
         <v>0.54800000000000004</v>
       </c>
       <c r="E27">
-        <f>AVERAGE(C27:D27)</f>
+        <f t="shared" si="0"/>
         <v>0.50900000000000001</v>
       </c>
       <c r="F27">
@@ -15373,7 +15377,7 @@
         <v>127.35615</v>
       </c>
       <c r="G27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>254.7123</v>
       </c>
     </row>
@@ -15391,7 +15395,7 @@
         <v>1.034</v>
       </c>
       <c r="E28">
-        <f>AVERAGE(C28:D28)</f>
+        <f t="shared" si="0"/>
         <v>1.0569999999999999</v>
       </c>
       <c r="F28">
@@ -15399,7 +15403,7 @@
         <v>201.67783999999997</v>
       </c>
       <c r="G28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>403.35567999999995</v>
       </c>
     </row>
@@ -15417,7 +15421,7 @@
         <v>0.41599999999999998</v>
       </c>
       <c r="E29">
-        <f>AVERAGE(C29:D29)</f>
+        <f t="shared" si="0"/>
         <v>0.40400000000000003</v>
       </c>
       <c r="F29">
@@ -15425,7 +15429,7 @@
         <v>75.50518000000001</v>
       </c>
       <c r="G29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>151.01036000000002</v>
       </c>
     </row>
@@ -15443,7 +15447,7 @@
         <v>0.60899999999999999</v>
       </c>
       <c r="E30">
-        <f>AVERAGE(C30:D30)</f>
+        <f t="shared" si="0"/>
         <v>0.55149999999999999</v>
       </c>
       <c r="F30">
@@ -15451,7 +15455,7 @@
         <v>104.00512999999999</v>
       </c>
       <c r="G30">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>208.01025999999999</v>
       </c>
     </row>
@@ -15469,7 +15473,7 @@
         <v>0.70899999999999996</v>
       </c>
       <c r="E31">
-        <f>AVERAGE(C31:D31)</f>
+        <f t="shared" si="0"/>
         <v>0.63849999999999996</v>
       </c>
       <c r="F31">
@@ -15477,7 +15481,7 @@
         <v>159.93187500000002</v>
       </c>
       <c r="G31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>319.86375000000004</v>
       </c>
     </row>
@@ -15495,7 +15499,7 @@
         <v>0.497</v>
       </c>
       <c r="E32">
-        <f>AVERAGE(C32:D32)</f>
+        <f t="shared" si="0"/>
         <v>0.52150000000000007</v>
       </c>
       <c r="F32">
@@ -15503,7 +15507,7 @@
         <v>130.50052500000004</v>
       </c>
       <c r="G32">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>261.00105000000008</v>
       </c>
     </row>
@@ -15521,7 +15525,7 @@
         <v>1.0509999999999999</v>
       </c>
       <c r="E33">
-        <f>AVERAGE(C33:D33)</f>
+        <f t="shared" si="0"/>
         <v>1.0634999999999999</v>
       </c>
       <c r="F33">
@@ -15529,7 +15533,7 @@
         <v>179.12225999999998</v>
       </c>
       <c r="G33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>358.24451999999997</v>
       </c>
     </row>
@@ -15547,7 +15551,7 @@
         <v>0.51100000000000001</v>
       </c>
       <c r="E34">
-        <f>AVERAGE(C34:D34)</f>
+        <f t="shared" ref="E34:E65" si="2">AVERAGE(C34:D34)</f>
         <v>0.45750000000000002</v>
       </c>
       <c r="F34">
@@ -15555,7 +15559,7 @@
         <v>87.312925000000007</v>
       </c>
       <c r="G34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>174.62585000000001</v>
       </c>
     </row>
@@ -15573,7 +15577,7 @@
         <v>0.56899999999999995</v>
       </c>
       <c r="E35">
-        <f>AVERAGE(C35:D35)</f>
+        <f t="shared" si="2"/>
         <v>0.54600000000000004</v>
       </c>
       <c r="F35">
@@ -15581,7 +15585,7 @@
         <v>102.94242000000001</v>
       </c>
       <c r="G35">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>205.88484000000003</v>
       </c>
     </row>
@@ -15599,7 +15603,7 @@
         <v>0.877</v>
       </c>
       <c r="E36">
-        <f>AVERAGE(C36:D36)</f>
+        <f t="shared" si="2"/>
         <v>0.76500000000000001</v>
       </c>
       <c r="F36">
@@ -15607,7 +15611,7 @@
         <v>152.59825000000001</v>
       </c>
       <c r="G36">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>305.19650000000001</v>
       </c>
     </row>
@@ -15625,7 +15629,7 @@
         <v>0.66</v>
       </c>
       <c r="E37">
-        <f>AVERAGE(C37:D37)</f>
+        <f t="shared" si="2"/>
         <v>0.71850000000000003</v>
       </c>
       <c r="F37">
@@ -15633,7 +15637,7 @@
         <v>136.27287000000001</v>
       </c>
       <c r="G37">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>272.54574000000002</v>
       </c>
     </row>
@@ -15651,7 +15655,7 @@
         <v>0.498</v>
       </c>
       <c r="E38">
-        <f>AVERAGE(C38:D38)</f>
+        <f t="shared" si="2"/>
         <v>0.46699999999999997</v>
       </c>
       <c r="F38">
@@ -15659,7 +15663,7 @@
         <v>87.678039999999996</v>
       </c>
       <c r="G38">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>175.35607999999999</v>
       </c>
     </row>
@@ -15677,7 +15681,7 @@
         <v>0.45700000000000002</v>
       </c>
       <c r="E39">
-        <f>AVERAGE(C39:D39)</f>
+        <f t="shared" si="2"/>
         <v>0.47299999999999998</v>
       </c>
       <c r="F39">
@@ -15685,7 +15689,7 @@
         <v>118.30034999999999</v>
       </c>
       <c r="G39">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>236.60069999999999</v>
       </c>
     </row>
@@ -15703,7 +15707,7 @@
         <v>0.61</v>
       </c>
       <c r="E40">
-        <f>AVERAGE(C40:D40)</f>
+        <f t="shared" si="2"/>
         <v>0.62850000000000006</v>
       </c>
       <c r="F40">
@@ -15711,7 +15715,7 @@
         <v>123.617935</v>
       </c>
       <c r="G40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>247.23587000000001</v>
       </c>
     </row>
@@ -15729,7 +15733,7 @@
         <v>0.54400000000000004</v>
       </c>
       <c r="E41">
-        <f>AVERAGE(C41:D41)</f>
+        <f t="shared" si="2"/>
         <v>0.504</v>
       </c>
       <c r="F41">
@@ -15737,7 +15741,7 @@
         <v>94.827179999999998</v>
       </c>
       <c r="G41">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>189.65436</v>
       </c>
     </row>
@@ -15755,7 +15759,7 @@
         <v>0.88600000000000001</v>
       </c>
       <c r="E42">
-        <f>AVERAGE(C42:D42)</f>
+        <f t="shared" si="2"/>
         <v>0.88800000000000001</v>
       </c>
       <c r="F42">
@@ -15763,7 +15767,7 @@
         <v>147.39888000000002</v>
       </c>
       <c r="G42">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>294.79776000000004</v>
       </c>
     </row>
@@ -15781,7 +15785,7 @@
         <v>0.90200000000000002</v>
       </c>
       <c r="E43">
-        <f>AVERAGE(C43:D43)</f>
+        <f t="shared" si="2"/>
         <v>0.78700000000000003</v>
       </c>
       <c r="F43">
@@ -15789,7 +15793,7 @@
         <v>197.28705000000002</v>
       </c>
       <c r="G43">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>394.57410000000004</v>
       </c>
     </row>
@@ -15807,7 +15811,7 @@
         <v>0.378</v>
       </c>
       <c r="E44">
-        <f>AVERAGE(C44:D44)</f>
+        <f t="shared" si="2"/>
         <v>0.39649999999999996</v>
       </c>
       <c r="F44">
@@ -15815,7 +15819,7 @@
         <v>74.056029999999993</v>
       </c>
       <c r="G44">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>148.11205999999999</v>
       </c>
     </row>
@@ -15833,7 +15837,7 @@
         <v>0.437</v>
       </c>
       <c r="E45">
-        <f>AVERAGE(C45:D45)</f>
+        <f t="shared" si="2"/>
         <v>0.437</v>
       </c>
       <c r="F45">
@@ -15841,7 +15845,7 @@
         <v>82.960570000000004</v>
       </c>
       <c r="G45">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>165.92114000000001</v>
       </c>
     </row>
@@ -15859,7 +15863,7 @@
         <v>0.32700000000000001</v>
       </c>
       <c r="E46">
-        <f>AVERAGE(C46:D46)</f>
+        <f t="shared" si="2"/>
         <v>0.28749999999999998</v>
       </c>
       <c r="F46">
@@ -15867,7 +15871,7 @@
         <v>38.852499999999992</v>
       </c>
       <c r="G46">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>77.704999999999984</v>
       </c>
     </row>
@@ -15885,7 +15889,7 @@
         <v>0.90100000000000002</v>
       </c>
       <c r="E47">
-        <f>AVERAGE(C47:D47)</f>
+        <f t="shared" si="2"/>
         <v>0.92749999999999999</v>
       </c>
       <c r="F47">
@@ -15893,7 +15897,7 @@
         <v>232.62982500000001</v>
       </c>
       <c r="G47">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>465.25965000000002</v>
       </c>
     </row>
@@ -15911,7 +15915,7 @@
         <v>1.1519999999999999</v>
       </c>
       <c r="E48">
-        <f>AVERAGE(C48:D48)</f>
+        <f t="shared" si="2"/>
         <v>1.1214499999999998</v>
       </c>
       <c r="F48">
@@ -15919,7 +15923,7 @@
         <v>228.27614949999997</v>
       </c>
       <c r="G48">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>456.55229899999995</v>
       </c>
     </row>
@@ -15937,7 +15941,7 @@
         <v>0.92300000000000004</v>
       </c>
       <c r="E49">
-        <f>AVERAGE(C49:D49)</f>
+        <f t="shared" si="2"/>
         <v>1.0994999999999999</v>
       </c>
       <c r="F49">
@@ -15945,7 +15949,7 @@
         <v>185.62961999999999</v>
       </c>
       <c r="G49">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>371.25923999999998</v>
       </c>
     </row>
@@ -15963,7 +15967,7 @@
         <v>0.55600000000000005</v>
       </c>
       <c r="E50">
-        <f>AVERAGE(C50:D50)</f>
+        <f t="shared" si="2"/>
         <v>0.52750000000000008</v>
       </c>
       <c r="F50">
@@ -15971,7 +15975,7 @@
         <v>132.00982500000003</v>
       </c>
       <c r="G50">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>264.01965000000007</v>
       </c>
     </row>
@@ -15989,7 +15993,7 @@
         <v>1.0009999999999999</v>
       </c>
       <c r="E51">
-        <f>AVERAGE(C51:D51)</f>
+        <f t="shared" si="2"/>
         <v>1.0274999999999999</v>
       </c>
       <c r="F51">
@@ -15997,7 +16001,7 @@
         <v>208.32962499999996</v>
       </c>
       <c r="G51">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>416.65924999999993</v>
       </c>
     </row>
@@ -16015,7 +16019,7 @@
         <v>0.39100000000000001</v>
       </c>
       <c r="E52">
-        <f>AVERAGE(C52:D52)</f>
+        <f t="shared" si="2"/>
         <v>0.25800000000000001</v>
       </c>
       <c r="F52">
@@ -16023,7 +16027,7 @@
         <v>33.52008</v>
       </c>
       <c r="G52">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>67.04016</v>
       </c>
     </row>
@@ -16041,7 +16045,7 @@
         <v>0.22</v>
       </c>
       <c r="E53">
-        <f>AVERAGE(C53:D53)</f>
+        <f t="shared" si="2"/>
         <v>0.21299999999999999</v>
       </c>
       <c r="F53">
@@ -16049,7 +16053,7 @@
         <v>35.403129999999997</v>
       </c>
       <c r="G53">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>70.806259999999995</v>
       </c>
     </row>
@@ -16067,7 +16071,7 @@
         <v>0.33500000000000002</v>
       </c>
       <c r="E54">
-        <f>AVERAGE(C54:D54)</f>
+        <f t="shared" si="2"/>
         <v>0.31950000000000001</v>
       </c>
       <c r="F54">
@@ -16075,7 +16079,7 @@
         <v>58.014144999999999</v>
       </c>
       <c r="G54">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>116.02829</v>
       </c>
     </row>
@@ -16093,7 +16097,7 @@
         <v>0.112</v>
       </c>
       <c r="E55">
-        <f>AVERAGE(C55:D55)</f>
+        <f t="shared" si="2"/>
         <v>0.10650000000000001</v>
       </c>
       <c r="F55">
@@ -16101,7 +16105,7 @@
         <v>26.107275000000005</v>
       </c>
       <c r="G55">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>52.21455000000001</v>
       </c>
     </row>
@@ -16119,15 +16123,15 @@
         <v>0.307</v>
       </c>
       <c r="E56">
-        <f>AVERAGE(C56:D56)</f>
+        <f t="shared" si="2"/>
         <v>0.31</v>
       </c>
       <c r="F56">
-        <f>212.31*E56-9.8189</f>
+        <f t="shared" ref="F56:F61" si="3">212.31*E56-9.8189</f>
         <v>55.997200000000007</v>
       </c>
       <c r="G56">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>111.99440000000001</v>
       </c>
     </row>
@@ -16145,15 +16149,15 @@
         <v>0.29599999999999999</v>
       </c>
       <c r="E57">
-        <f>AVERAGE(C57:D57)</f>
+        <f t="shared" si="2"/>
         <v>0.28800000000000003</v>
       </c>
       <c r="F57">
-        <f>212.31*E57-9.8189</f>
+        <f t="shared" si="3"/>
         <v>51.326380000000007</v>
       </c>
       <c r="G57">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>102.65276000000001</v>
       </c>
     </row>
@@ -16171,15 +16175,15 @@
         <v>0.38500000000000001</v>
       </c>
       <c r="E58">
-        <f>AVERAGE(C58:D58)</f>
+        <f t="shared" si="2"/>
         <v>0.40500000000000003</v>
       </c>
       <c r="F58">
-        <f>212.31*E58-9.8189</f>
+        <f t="shared" si="3"/>
         <v>76.166650000000004</v>
       </c>
       <c r="G58">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>152.33330000000001</v>
       </c>
     </row>
@@ -16197,15 +16201,15 @@
         <v>0.19</v>
       </c>
       <c r="E59">
-        <f>AVERAGE(C59:D59)</f>
+        <f t="shared" si="2"/>
         <v>0.17849999999999999</v>
       </c>
       <c r="F59">
-        <f>212.31*E59-9.8189</f>
+        <f t="shared" si="3"/>
         <v>28.078434999999999</v>
       </c>
       <c r="G59">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>56.156869999999998</v>
       </c>
     </row>
@@ -16223,15 +16227,15 @@
         <v>0.56200000000000006</v>
       </c>
       <c r="E60">
-        <f>AVERAGE(C60:D60)</f>
+        <f t="shared" si="2"/>
         <v>0.52400000000000002</v>
       </c>
       <c r="F60">
-        <f>212.31*E60-9.8189</f>
+        <f t="shared" si="3"/>
         <v>101.43154000000001</v>
       </c>
       <c r="G60">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>202.86308000000002</v>
       </c>
     </row>
@@ -16249,15 +16253,15 @@
         <v>0.23599999999999999</v>
       </c>
       <c r="E61">
-        <f>AVERAGE(C61:D61)</f>
+        <f t="shared" si="2"/>
         <v>0.27700000000000002</v>
       </c>
       <c r="F61">
-        <f>212.31*E61-9.8189</f>
+        <f t="shared" si="3"/>
         <v>48.990970000000004</v>
       </c>
       <c r="G61">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>97.981940000000009</v>
       </c>
     </row>
@@ -16275,7 +16279,7 @@
         <v>0.69599999999999995</v>
       </c>
       <c r="E62">
-        <f>AVERAGE(C62:D62)</f>
+        <f t="shared" si="2"/>
         <v>0.65349999999999997</v>
       </c>
       <c r="F62">
@@ -16283,7 +16287,7 @@
         <v>105.01065999999999</v>
       </c>
       <c r="G62">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>210.02131999999997</v>
       </c>
     </row>
@@ -16301,7 +16305,7 @@
         <v>0.214</v>
       </c>
       <c r="E63">
-        <f>AVERAGE(C63:D63)</f>
+        <f t="shared" si="2"/>
         <v>0.21099999999999999</v>
       </c>
       <c r="F63">
@@ -16309,7 +16313,7 @@
         <v>34.97851</v>
       </c>
       <c r="G63">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>69.95702</v>
       </c>
     </row>
@@ -16327,7 +16331,7 @@
         <v>0.186</v>
       </c>
       <c r="E64">
-        <f>AVERAGE(C64:D64)</f>
+        <f t="shared" si="2"/>
         <v>0.18</v>
       </c>
       <c r="F64">
@@ -16335,11 +16339,11 @@
         <v>28.396900000000002</v>
       </c>
       <c r="G64">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>56.793800000000005</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A65">
         <v>265</v>
       </c>
@@ -16353,7 +16357,7 @@
         <v>0.36699999999999999</v>
       </c>
       <c r="E65">
-        <f>AVERAGE(C65:D65)</f>
+        <f t="shared" si="2"/>
         <v>0.33350000000000002</v>
       </c>
       <c r="F65">
@@ -16361,11 +16365,11 @@
         <v>47.167459999999998</v>
       </c>
       <c r="G65">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>94.334919999999997</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A66">
         <v>268</v>
       </c>
@@ -16379,7 +16383,7 @@
         <v>0.56000000000000005</v>
       </c>
       <c r="E66">
-        <f>AVERAGE(C66:D66)</f>
+        <f t="shared" ref="E66:E97" si="4">AVERAGE(C66:D66)</f>
         <v>0.51350000000000007</v>
       </c>
       <c r="F66">
@@ -16387,11 +16391,11 @@
         <v>99.202285000000018</v>
       </c>
       <c r="G66">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>198.40457000000004</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A67">
         <v>269</v>
       </c>
@@ -16405,7 +16409,7 @@
         <v>1.08</v>
       </c>
       <c r="E67">
-        <f>AVERAGE(C67:D67)</f>
+        <f t="shared" si="4"/>
         <v>1.0630000000000002</v>
       </c>
       <c r="F67">
@@ -16413,11 +16417,14 @@
         <v>215.86663000000004</v>
       </c>
       <c r="G67">
-        <f t="shared" ref="G67:G116" si="1">F67*2</f>
+        <f t="shared" ref="G67:G116" si="5">F67*2</f>
         <v>431.73326000000009</v>
       </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="I67" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A68">
         <v>270</v>
       </c>
@@ -16431,7 +16438,7 @@
         <v>0.28599999999999998</v>
       </c>
       <c r="E68">
-        <f>AVERAGE(C68:D68)</f>
+        <f t="shared" si="4"/>
         <v>0.28149999999999997</v>
       </c>
       <c r="F68">
@@ -16439,11 +16446,11 @@
         <v>49.946364999999993</v>
       </c>
       <c r="G68">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>99.892729999999986</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A69">
         <v>271</v>
       </c>
@@ -16457,7 +16464,7 @@
         <v>1.0820000000000001</v>
       </c>
       <c r="E69">
-        <f>AVERAGE(C69:D69)</f>
+        <f t="shared" si="4"/>
         <v>1.0335000000000001</v>
       </c>
       <c r="F69">
@@ -16465,11 +16472,11 @@
         <v>209.60348500000003</v>
       </c>
       <c r="G69">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>419.20697000000007</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A70">
         <v>272</v>
       </c>
@@ -16483,7 +16490,7 @@
         <v>0.77500000000000002</v>
       </c>
       <c r="E70">
-        <f>AVERAGE(C70:D70)</f>
+        <f t="shared" si="4"/>
         <v>0.77849999999999997</v>
       </c>
       <c r="F70">
@@ -16491,11 +16498,11 @@
         <v>155.46443499999998</v>
       </c>
       <c r="G70">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>310.92886999999996</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A71">
         <v>273</v>
       </c>
@@ -16509,7 +16516,7 @@
         <v>1.605</v>
       </c>
       <c r="E71">
-        <f>AVERAGE(C71:D71)</f>
+        <f t="shared" si="4"/>
         <v>1.5445</v>
       </c>
       <c r="F71">
@@ -16517,11 +16524,11 @@
         <v>266.06781999999998</v>
       </c>
       <c r="G71">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>532.13563999999997</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A72">
         <v>274</v>
       </c>
@@ -16535,7 +16542,7 @@
         <v>0.54900000000000004</v>
       </c>
       <c r="E72">
-        <f>AVERAGE(C72:D72)</f>
+        <f t="shared" si="4"/>
         <v>0.63400000000000001</v>
       </c>
       <c r="F72">
@@ -16543,11 +16550,11 @@
         <v>124.78564000000001</v>
       </c>
       <c r="G72">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>249.57128000000003</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A73">
         <v>275</v>
       </c>
@@ -16561,7 +16568,7 @@
         <v>1.252</v>
       </c>
       <c r="E73">
-        <f>AVERAGE(C73:D73)</f>
+        <f t="shared" si="4"/>
         <v>1.2375</v>
       </c>
       <c r="F73">
@@ -16569,11 +16576,11 @@
         <v>210.5745</v>
       </c>
       <c r="G73">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>421.149</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A74">
         <v>276</v>
       </c>
@@ -16587,7 +16594,7 @@
         <v>1.3520000000000001</v>
       </c>
       <c r="E74">
-        <f>AVERAGE(C74:D74)</f>
+        <f t="shared" si="4"/>
         <v>1.3445</v>
       </c>
       <c r="F74">
@@ -16595,11 +16602,11 @@
         <v>275.63189500000004</v>
       </c>
       <c r="G74">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>551.26379000000009</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A75">
         <v>277</v>
       </c>
@@ -16613,7 +16620,7 @@
         <v>0.81399999999999995</v>
       </c>
       <c r="E75">
-        <f>AVERAGE(C75:D75)</f>
+        <f t="shared" si="4"/>
         <v>0.8254999999999999</v>
       </c>
       <c r="F75">
@@ -16621,11 +16628,11 @@
         <v>165.44300499999997</v>
       </c>
       <c r="G75">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>330.88600999999994</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A76">
         <v>278</v>
       </c>
@@ -16639,19 +16646,19 @@
         <v>1.3220000000000001</v>
       </c>
       <c r="E76">
-        <f>AVERAGE(C76:D76)</f>
+        <f t="shared" si="4"/>
         <v>1.111</v>
       </c>
       <c r="F76">
-        <f>251.55*E76-0.6828</f>
+        <f t="shared" ref="F76:F86" si="6">251.55*E76-0.6828</f>
         <v>278.78925000000004</v>
       </c>
       <c r="G76">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>557.57850000000008</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A77">
         <v>279</v>
       </c>
@@ -16665,19 +16672,19 @@
         <v>0.879</v>
       </c>
       <c r="E77">
-        <f>AVERAGE(C77:D77)</f>
+        <f t="shared" si="4"/>
         <v>0.84299999999999997</v>
       </c>
       <c r="F77">
-        <f>251.55*E77-0.6828</f>
+        <f t="shared" si="6"/>
         <v>211.37385</v>
       </c>
       <c r="G77">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>422.74770000000001</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A78">
         <v>280</v>
       </c>
@@ -16691,19 +16698,19 @@
         <v>0.64700000000000002</v>
       </c>
       <c r="E78">
-        <f>AVERAGE(C78:D78)</f>
+        <f t="shared" si="4"/>
         <v>0.61699999999999999</v>
       </c>
       <c r="F78">
-        <f>251.55*E78-0.6828</f>
+        <f t="shared" si="6"/>
         <v>154.52355000000003</v>
       </c>
       <c r="G78">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>309.04710000000006</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A79">
         <v>281</v>
       </c>
@@ -16717,19 +16724,19 @@
         <v>0.53800000000000003</v>
       </c>
       <c r="E79">
-        <f>AVERAGE(C79:D79)</f>
+        <f t="shared" si="4"/>
         <v>0.49250000000000005</v>
       </c>
       <c r="F79">
-        <f>251.55*E79-0.6828</f>
+        <f t="shared" si="6"/>
         <v>123.20557500000002</v>
       </c>
       <c r="G79">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>246.41115000000005</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A80">
         <v>282</v>
       </c>
@@ -16743,15 +16750,15 @@
         <v>0.71399999999999997</v>
       </c>
       <c r="E80">
-        <f>AVERAGE(C80:D80)</f>
+        <f t="shared" si="4"/>
         <v>0.69550000000000001</v>
       </c>
       <c r="F80">
-        <f>251.55*E80-0.6828</f>
+        <f t="shared" si="6"/>
         <v>174.27022500000001</v>
       </c>
       <c r="G80">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>348.54045000000002</v>
       </c>
     </row>
@@ -16769,15 +16776,15 @@
         <v>0.70099999999999996</v>
       </c>
       <c r="E81">
-        <f>AVERAGE(C81:D81)</f>
+        <f t="shared" si="4"/>
         <v>0.70849999999999991</v>
       </c>
       <c r="F81">
-        <f>251.55*E81-0.6828</f>
+        <f t="shared" si="6"/>
         <v>177.54037500000001</v>
       </c>
       <c r="G81">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>355.08075000000002</v>
       </c>
     </row>
@@ -16795,15 +16802,15 @@
         <v>0.73499999999999999</v>
       </c>
       <c r="E82">
-        <f>AVERAGE(C82:D82)</f>
+        <f t="shared" si="4"/>
         <v>0.69350000000000001</v>
       </c>
       <c r="F82">
-        <f>251.55*E82-0.6828</f>
+        <f t="shared" si="6"/>
         <v>173.76712500000002</v>
       </c>
       <c r="G82">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>347.53425000000004</v>
       </c>
     </row>
@@ -16821,15 +16828,15 @@
         <v>6</v>
       </c>
       <c r="E83">
-        <f>AVERAGE(C83:D83)</f>
+        <f t="shared" si="4"/>
         <v>1.1679999999999999</v>
       </c>
       <c r="F83">
-        <f>251.55*E83-0.6828</f>
+        <f t="shared" si="6"/>
         <v>293.12760000000003</v>
       </c>
       <c r="G83">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>586.25520000000006</v>
       </c>
     </row>
@@ -16847,15 +16854,15 @@
         <v>0.57599999999999996</v>
       </c>
       <c r="E84">
-        <f>AVERAGE(C84:D84)</f>
+        <f t="shared" si="4"/>
         <v>0.61</v>
       </c>
       <c r="F84">
-        <f>251.55*E84-0.6828</f>
+        <f t="shared" si="6"/>
         <v>152.76270000000002</v>
       </c>
       <c r="G84">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>305.52540000000005</v>
       </c>
     </row>
@@ -16873,15 +16880,15 @@
         <v>0.748</v>
       </c>
       <c r="E85">
-        <f>AVERAGE(C85:D85)</f>
+        <f t="shared" si="4"/>
         <v>0.69</v>
       </c>
       <c r="F85">
-        <f>251.55*E85-0.6828</f>
+        <f t="shared" si="6"/>
         <v>172.88670000000002</v>
       </c>
       <c r="G85">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>345.77340000000004</v>
       </c>
     </row>
@@ -16899,15 +16906,15 @@
         <v>0.53300000000000003</v>
       </c>
       <c r="E86">
-        <f>AVERAGE(C86:D86)</f>
+        <f t="shared" si="4"/>
         <v>0.42900000000000005</v>
       </c>
       <c r="F86">
-        <f>251.55*E86-0.6828</f>
+        <f t="shared" si="6"/>
         <v>107.23215000000002</v>
       </c>
       <c r="G86">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>214.46430000000004</v>
       </c>
     </row>
@@ -16925,7 +16932,7 @@
         <v>2.0169999999999999</v>
       </c>
       <c r="E87">
-        <f>AVERAGE(C87:D87)</f>
+        <f t="shared" si="4"/>
         <v>2.0209999999999999</v>
       </c>
       <c r="F87">
@@ -16933,7 +16940,7 @@
         <v>352.19995999999998</v>
       </c>
       <c r="G87">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>704.39991999999995</v>
       </c>
     </row>
@@ -16951,7 +16958,7 @@
         <v>0.71399999999999997</v>
       </c>
       <c r="E88">
-        <f>AVERAGE(C88:D88)</f>
+        <f t="shared" si="4"/>
         <v>0.61</v>
       </c>
       <c r="F88">
@@ -16959,7 +16966,7 @@
         <v>97.147599999999997</v>
       </c>
       <c r="G88">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>194.29519999999999</v>
       </c>
     </row>
@@ -16977,7 +16984,7 @@
         <v>1.048</v>
       </c>
       <c r="E89">
-        <f>AVERAGE(C89:D89)</f>
+        <f t="shared" si="4"/>
         <v>1.026</v>
       </c>
       <c r="F89">
@@ -16985,7 +16992,7 @@
         <v>208.01116000000002</v>
       </c>
       <c r="G89">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>416.02232000000004</v>
       </c>
     </row>
@@ -17003,7 +17010,7 @@
         <v>1.69</v>
       </c>
       <c r="E90">
-        <f>AVERAGE(C90:D90)</f>
+        <f t="shared" si="4"/>
         <v>1.6775</v>
       </c>
       <c r="F90">
@@ -17011,7 +17018,7 @@
         <v>290.10890000000001</v>
       </c>
       <c r="G90">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>580.21780000000001</v>
       </c>
     </row>
@@ -17029,7 +17036,7 @@
         <v>1.1319999999999999</v>
       </c>
       <c r="E91">
-        <f>AVERAGE(C91:D91)</f>
+        <f t="shared" si="4"/>
         <v>1.1859999999999999</v>
       </c>
       <c r="F91">
@@ -17037,7 +17044,7 @@
         <v>241.98075999999998</v>
       </c>
       <c r="G91">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>483.96151999999995</v>
       </c>
     </row>
@@ -17055,7 +17062,7 @@
         <v>0.99399999999999999</v>
       </c>
       <c r="E92">
-        <f>AVERAGE(C92:D92)</f>
+        <f t="shared" si="4"/>
         <v>0.95650000000000002</v>
       </c>
       <c r="F92">
@@ -17063,7 +17070,7 @@
         <v>239.92477500000004</v>
       </c>
       <c r="G92">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>479.84955000000008</v>
       </c>
     </row>
@@ -17081,7 +17088,7 @@
         <v>0.81299999999999994</v>
       </c>
       <c r="E93">
-        <f>AVERAGE(C93:D93)</f>
+        <f t="shared" si="4"/>
         <v>0.92649999999999999</v>
       </c>
       <c r="F93">
@@ -17089,7 +17096,7 @@
         <v>232.37827500000003</v>
       </c>
       <c r="G93">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>464.75655000000006</v>
       </c>
     </row>
@@ -17107,7 +17114,7 @@
         <v>1.823</v>
       </c>
       <c r="E94">
-        <f>AVERAGE(C94:D94)</f>
+        <f t="shared" si="4"/>
         <v>1.8399999999999999</v>
       </c>
       <c r="F94">
@@ -17115,7 +17122,7 @@
         <v>319.48239999999998</v>
       </c>
       <c r="G94">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>638.96479999999997</v>
       </c>
     </row>
@@ -17133,7 +17140,7 @@
         <v>1.8560000000000001</v>
       </c>
       <c r="E95">
-        <f>AVERAGE(C95:D95)</f>
+        <f t="shared" si="4"/>
         <v>1.8959999999999999</v>
       </c>
       <c r="F95">
@@ -17141,7 +17148,7 @@
         <v>392.72086000000002</v>
       </c>
       <c r="G95">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>785.44172000000003</v>
       </c>
     </row>
@@ -17159,7 +17166,7 @@
         <v>1.4119999999999999</v>
       </c>
       <c r="E96">
-        <f>AVERAGE(C96:D96)</f>
+        <f t="shared" si="4"/>
         <v>1.448</v>
       </c>
       <c r="F96">
@@ -17167,7 +17174,7 @@
         <v>248.62448000000001</v>
       </c>
       <c r="G96">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>497.24896000000001</v>
       </c>
     </row>
@@ -17185,7 +17192,7 @@
         <v>1.4430000000000001</v>
       </c>
       <c r="E97">
-        <f>AVERAGE(C97:D97)</f>
+        <f t="shared" si="4"/>
         <v>1.3565</v>
       </c>
       <c r="F97">
@@ -17193,7 +17200,7 @@
         <v>232.08494000000002</v>
       </c>
       <c r="G97">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>464.16988000000003</v>
       </c>
     </row>
@@ -17211,7 +17218,7 @@
         <v>0.9</v>
       </c>
       <c r="E98">
-        <f>AVERAGE(C98:D98)</f>
+        <f t="shared" ref="E98:E129" si="7">AVERAGE(C98:D98)</f>
         <v>0.74649999999999994</v>
       </c>
       <c r="F98">
@@ -17219,7 +17226,7 @@
         <v>141.68302999999997</v>
       </c>
       <c r="G98">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>283.36605999999995</v>
       </c>
     </row>
@@ -17237,7 +17244,7 @@
         <v>0.80300000000000005</v>
       </c>
       <c r="E99">
-        <f>AVERAGE(C99:D99)</f>
+        <f t="shared" si="7"/>
         <v>0.88549999999999995</v>
       </c>
       <c r="F99">
@@ -17245,7 +17252,7 @@
         <v>222.06472500000001</v>
       </c>
       <c r="G99">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>444.12945000000002</v>
       </c>
     </row>
@@ -17263,7 +17270,7 @@
         <v>0.48699999999999999</v>
       </c>
       <c r="E100">
-        <f>AVERAGE(C100:D100)</f>
+        <f t="shared" si="7"/>
         <v>0.42149999999999999</v>
       </c>
       <c r="F100">
@@ -17271,7 +17278,7 @@
         <v>105.34552499999999</v>
       </c>
       <c r="G100">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>210.69104999999999</v>
       </c>
     </row>
@@ -17289,7 +17296,7 @@
         <v>0.57899999999999996</v>
       </c>
       <c r="E101">
-        <f>AVERAGE(C101:D101)</f>
+        <f t="shared" si="7"/>
         <v>0.56400000000000006</v>
       </c>
       <c r="F101">
@@ -17297,7 +17304,7 @@
         <v>141.19140000000004</v>
       </c>
       <c r="G101">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>282.38280000000009</v>
       </c>
     </row>
@@ -17315,7 +17322,7 @@
         <v>0.92800000000000005</v>
       </c>
       <c r="E102">
-        <f>AVERAGE(C102:D102)</f>
+        <f t="shared" si="7"/>
         <v>0.9375</v>
       </c>
       <c r="F102">
@@ -17323,7 +17330,7 @@
         <v>189.22172499999999</v>
       </c>
       <c r="G102">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>378.44344999999998</v>
       </c>
     </row>
@@ -17341,7 +17348,7 @@
         <v>1.3720000000000001</v>
       </c>
       <c r="E103">
-        <f>AVERAGE(C103:D103)</f>
+        <f t="shared" si="7"/>
         <v>1.278</v>
       </c>
       <c r="F103">
@@ -17349,7 +17356,7 @@
         <v>217.89528000000001</v>
       </c>
       <c r="G103">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>435.79056000000003</v>
       </c>
     </row>
@@ -17367,7 +17374,7 @@
         <v>1.4550000000000001</v>
       </c>
       <c r="E104">
-        <f>AVERAGE(C104:D104)</f>
+        <f t="shared" si="7"/>
         <v>1.4140000000000001</v>
       </c>
       <c r="F104">
@@ -17375,7 +17382,7 @@
         <v>290.38744000000003</v>
       </c>
       <c r="G104">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>580.77488000000005</v>
       </c>
     </row>
@@ -17393,7 +17400,7 @@
         <v>0.64400000000000002</v>
       </c>
       <c r="E105">
-        <f>AVERAGE(C105:D105)</f>
+        <f t="shared" si="7"/>
         <v>0.61749999999999994</v>
       </c>
       <c r="F105">
@@ -17401,7 +17408,7 @@
         <v>154.649325</v>
       </c>
       <c r="G105">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>309.29865000000001</v>
       </c>
     </row>
@@ -17419,7 +17426,7 @@
         <v>1.079</v>
       </c>
       <c r="E106">
-        <f>AVERAGE(C106:D106)</f>
+        <f t="shared" si="7"/>
         <v>1.1945000000000001</v>
       </c>
       <c r="F106">
@@ -17427,7 +17434,7 @@
         <v>202.80182000000002</v>
       </c>
       <c r="G106">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>405.60364000000004</v>
       </c>
     </row>
@@ -17445,7 +17452,7 @@
         <v>1.2929999999999999</v>
       </c>
       <c r="E107">
-        <f>AVERAGE(C107:D107)</f>
+        <f t="shared" si="7"/>
         <v>1.2829999999999999</v>
       </c>
       <c r="F107">
@@ -17453,7 +17460,7 @@
         <v>218.79907999999995</v>
       </c>
       <c r="G107">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>437.59815999999989</v>
       </c>
     </row>
@@ -17471,7 +17478,7 @@
         <v>0.83399999999999996</v>
       </c>
       <c r="E108">
-        <f>AVERAGE(C108:D108)</f>
+        <f t="shared" si="7"/>
         <v>0.76600000000000001</v>
       </c>
       <c r="F108">
@@ -17479,7 +17486,7 @@
         <v>152.81056000000001</v>
       </c>
       <c r="G108">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>305.62112000000002</v>
       </c>
     </row>
@@ -17497,7 +17504,7 @@
         <v>8.8999999999999996E-2</v>
       </c>
       <c r="E109">
-        <f>AVERAGE(C109:D109)</f>
+        <f t="shared" si="7"/>
         <v>7.4499999999999997E-2</v>
       </c>
       <c r="F109">
@@ -17505,7 +17512,7 @@
         <v>5.9981950000000008</v>
       </c>
       <c r="G109">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>11.996390000000002</v>
       </c>
     </row>
@@ -17523,7 +17530,7 @@
         <v>9.0999999999999998E-2</v>
       </c>
       <c r="E110">
-        <f>AVERAGE(C110:D110)</f>
+        <f t="shared" si="7"/>
         <v>9.8500000000000004E-2</v>
       </c>
       <c r="F110">
@@ -17531,7 +17538,7 @@
         <v>11.093635000000003</v>
       </c>
       <c r="G110">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>22.187270000000005</v>
       </c>
     </row>
@@ -17549,7 +17556,7 @@
         <v>4.5999999999999999E-2</v>
       </c>
       <c r="E111">
-        <f>AVERAGE(C111:D111)</f>
+        <f t="shared" si="7"/>
         <v>4.5999999999999999E-2</v>
       </c>
       <c r="F111">
@@ -17557,7 +17564,7 @@
         <v>10.888500000000001</v>
       </c>
       <c r="G111">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>21.777000000000001</v>
       </c>
     </row>
@@ -17575,7 +17582,7 @@
         <v>5.8000000000000003E-2</v>
       </c>
       <c r="E112">
-        <f>AVERAGE(C112:D112)</f>
+        <f t="shared" si="7"/>
         <v>6.0499999999999998E-2</v>
       </c>
       <c r="F112">
@@ -17583,7 +17590,7 @@
         <v>9.1341099999999997</v>
       </c>
       <c r="G112">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>18.268219999999999</v>
       </c>
     </row>
@@ -17601,7 +17608,7 @@
         <v>6.6000000000000003E-2</v>
       </c>
       <c r="E113">
-        <f>AVERAGE(C113:D113)</f>
+        <f t="shared" si="7"/>
         <v>5.3000000000000005E-2</v>
       </c>
       <c r="F113">
@@ -17609,7 +17616,7 @@
         <v>12.649350000000002</v>
       </c>
       <c r="G113">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>25.298700000000004</v>
       </c>
     </row>
@@ -17627,7 +17634,7 @@
         <v>0.112</v>
       </c>
       <c r="E114">
-        <f>AVERAGE(C114:D114)</f>
+        <f t="shared" si="7"/>
         <v>0.112</v>
       </c>
       <c r="F114">
@@ -17635,7 +17642,7 @@
         <v>7.1291200000000003</v>
       </c>
       <c r="G114">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>14.258240000000001</v>
       </c>
     </row>
@@ -17653,7 +17660,7 @@
         <v>4.5999999999999999E-2</v>
       </c>
       <c r="E115">
-        <f>AVERAGE(C115:D115)</f>
+        <f t="shared" si="7"/>
         <v>5.2999999999999999E-2</v>
       </c>
       <c r="F115">
@@ -17661,7 +17668,7 @@
         <v>1.4335300000000011</v>
       </c>
       <c r="G115">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>2.8670600000000022</v>
       </c>
     </row>
@@ -17679,7 +17686,7 @@
         <v>9.0999999999999998E-2</v>
       </c>
       <c r="E116">
-        <f>AVERAGE(C116:D116)</f>
+        <f t="shared" si="7"/>
         <v>7.3999999999999996E-2</v>
       </c>
       <c r="F116">
@@ -17687,7 +17694,7 @@
         <v>17.931899999999999</v>
       </c>
       <c r="G116">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>35.863799999999998</v>
       </c>
     </row>
@@ -17946,4 +17953,18 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{378B9C58-5373-479F-A8C1-E2B115C0B69D}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>